<commit_message>
Initial Dropbox-based sync and cleanup
</commit_message>
<xml_diff>
--- a/General Utilities/General Utlities.xlsx
+++ b/General Utilities/General Utlities.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profmc/Library/CloudStorage/Dropbox/Lambda-Update-Project/Lambda-Development/General Utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a47027c9c1b1b6a/Documents/GitHub/Lambda-Development/General Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCE266A-C6E4-AF47-9DAC-B6B63284E2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{8FCE266A-C6E4-AF47-9DAC-B6B63284E2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FAEECE-20C2-49D5-BD46-97F1D688F373}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="2380" windowWidth="33260" windowHeight="14260" xr2:uid="{7A445647-2974-6942-9320-70750788AE91}"/>
+    <workbookView xWindow="615" yWindow="2010" windowWidth="28185" windowHeight="14190" xr2:uid="{7A445647-2974-6942-9320-70750788AE91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="COUNTA_STRICT">_xlfn.LAMBDA(_xlpm.input, IF(COUNTIF(_xlpm.input, "*?") = 0, 0, COUNTA(_xlpm.input)))</definedName>
     <definedName name="FORMULA_TEXT">_xlfn.LAMBDA(_xlpm.formula_cell, _xlfn.LET(_xlpm.raw, _xlfn.FORMULATEXT(_xlpm.formula_cell), _xlpm.clean, _xlfn.TEXTAFTER(_xlpm.raw, "="), _xlpm.label, SUBSTITUTE(CELL("address", _xlpm.formula_cell), "$", "") &amp; ":= ", _xlpm.label &amp; _xlpm.clean))</definedName>
     <definedName name="FRAC">_xlfn.LAMBDA(_xlpm.input,_xlop.mode, _xlfn.LET(_xlpm.mode, IF(OR(_xlfn.ISOMITTED(_xlpm.mode), _xlpm.mode &gt; 1), 0, _xlpm.mode), _xlpm.frac_part, _xlpm.input - TRUNC(_xlpm.input), IF(_xlpm.mode = 1, _xlpm.frac_part, ABS(_xlpm.frac_part))))</definedName>
     <definedName name="RECIP">_xlfn.LAMBDA(_xlpm.input, 1 / _xlpm.input)</definedName>
@@ -67,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.00000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -99,7 +100,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +435,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -466,18 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6503EE-3967-F142-A914-D59AF539BB00}">
-  <dimension ref="B3:D27"/>
+  <dimension ref="B3:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
@@ -572,7 +573,13 @@
         <v>B14:= FORMULA_TEXT(B14)</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
+    <row r="18" spans="2:6">
+      <c r="F18" cm="1">
+        <f t="array" aca="1" ref="F18" ca="1">COUNTA_STRICT(D3:D14)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
       <c r="B27" s="1"/>
     </row>
   </sheetData>
@@ -581,7 +588,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABSAEUAQwBJAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAYwBpAHAAcgBvAGMAYQBsACAAKABtAHUAbAB0AGkAcABsAGkAYwBhAHQAaQB2AGUAIABpAG4AdgBlAHIAcwBlACkAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAaQBuAGcAbABlACAAZABlAGMAaQBtAGEAbAAgAHYAYQBsAHUAZQAgAGUAcQB1AGEAbAAgAHQAbwAgADEAIABkAGkAdgBpAGQAZQBkACAAYgB5ACAAdABoAGUAIABpAG4AcAB1AHQALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAbgB5ACAAbgBvAG4AegBlAHIAbwAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAHQAdQByAG4AcwAgAGAAIwBEAEkAVgAvADAAIQBgACAAaQBmACAAaQBuAHAAdQB0ACAAaQBzACAAegBlAHIAbwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGYAbABpAHAAcABpAG4AZwAgAGYAcgBhAGMAdABpAG8AbgBzACwAIABjAG8AbgB2AGUAcgB0AGkAbgBnACAAcgBhAHQAZQBzACAAKABlAC4AZwAuACwAIABIAHoAIACUISAAcwBlAGMAbwBuAGQAcwApACwAIABvAHIAIABpAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGkAbwBzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAA0ACkAIACSISAAMAAuADIANQBcAG4AIAAgACAAIAAgAFIARQBDAEkAUAAoADAALgAyACkAIACSISAANQBcAG4AKgAvAFwAbgBcAG4AXABuAFIARQBDAEkAUAAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAAMQAgAC8AIABpAG4AcAB1AHQAKQA7AFwAbgBcAG4ALwAqACAARgBSAEEAQwA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIAAoAG4AbwBuAC0AaQBuAHQAZQBnAGUAcgApACAAcABhAHIAdAAgAG8AZgAgAGEAIABuAHUAbQBiAGUAcgAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAcwBjAGEAbABhAHIAIABkAGUAYwBpAG0AYQBsACAAYgBlAHQAdwBlAGUAbgAgADAAIABhAG4AZAAgADEAIAAoAG8AcgAgAC0AMQAgAGEAbgBkACAAMAAgAGkAZgAgAHMAaQBnAG4AIABpAHMAIABwAHIAZQBzAGUAcgB2AGUAZAApAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABpAG4AcAB1AHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABUAGgAZQAgAG4AdQBtAGIAZQByACAAdABvACAAZQB4AHQAcgBhAGMAdAAgAHQAaABlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABmAHIAbwBtAC4AXABuACAAIAAgAC0AIABtAG8AZABlACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATwB1AHQAcAB1AHQAIABtAG8AZABlACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAMAA6ACAAQQBsAHcAYQB5AHMAIAByAGUAdAB1AHIAbgAgAHAAbwBzAGkAdABpAHYAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0AFwAbgAgACAAIAAgACAAIAAgAC0AIAAxADoAIABQAHIAZQBzAGUAcgB2AGUAIABzAGkAZwBuACAAbwBmACAAaQBuAHAAdQB0ACAAKABlAC4AZwAuACwAIAAtADMALgAyADUAIACSISAALQAwAC4AMgA1ACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAEMAbwBtAHAAbABlAG0AZQBuAHQAcwAgAEUAeABjAGUAbAAZIHMAIABUAFIAVQBOAEMAIABhAG4AZAAgAFEAVQBPAFQASQBFAE4AVAAgAGYAdQBuAGMAdABpAG8AbgBzAC4AXABuACAAIAAgAC0AIABVAHMAZQBmAHUAbAAgAGYAbwByACAAZABlAHQAZQBjAHQAaQBuAGcAIABkAGUAYwBpAG0AYQBsACAAcgBlAG0AYQBpAG4AZABlAHIAcwAgAGEAbgBkACAAYQBuAGEAbAB5AHoAaQBuAGcAIABvAGYAZgBzAGUAdABzACAAZgByAG8AbQAgAHcAaABvAGwAZQAgAHYAYQBsAHUAZQBzAC4AXABuACAAIAAgAC0AIABTAGkAZwBuAC0AcAByAGUAcwBlAHIAdgBpAG4AZwAgAG0AbwBkAGUAIABjAGEAbgAgAGkAbgBkAGkAYwBhAHQAZQAgAHcAaABlAHQAaABlAHIAIABhACAAdgBhAGwAdQBlACAAaQBzACAAagB1AHMAdAAgAGEAYgBvAHYAZQAgAG8AcgAgAGoAdQBzAHQAIABiAGUAbABvAHcAIABhAG4AIABpAG4AdABlAGcAZQByAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlAHMAOgBcAG4AIAAgACAARgBSAEEAQwAoAC0AMwAuADIANQApACAAIAAgACAAIAAgACAAkiEgADAALgAyADUAIAAgAFwAbgAgACAAIABGAFIAQQBDACgALQAzAC4AMgA1ACwAIAAxACkAIAAgACAAIACSISAALQAwAC4AMgA1AFwAbgAqAC8AXABuAFwAbgBcAG4ARgBSAEEAQwAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARABlAGYAYQB1AGwAdAAgAG0AbwBkAGUAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAGkAbgB2AGEAbABpAGQAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGIAeQAgAHMAdQBiAHQAcgBhAGMAdABpAG4AZwAgAGkAbgB0AGUAZwBlAHIAIABwAG8AcgB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAAZgByAGEAYwBfAHAAYQByAHQALAAgAGkAbgBwAHUAdAAgAC0AIABUAFIAVQBOAEMAKABpAG4AcAB1AHQAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAZQB0AHUAcgBuACAAcwBpAGcAbgBlAGQAIABvAHIAIABhAGIAcwBvAGwAdQB0AGUAIAB2AGEAbAB1AGUAIABkAGUAcABlAG4AZABpAG4AZwAgAG8AbgAgAG0AbwBkAGUAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlACAAPQAgADEALAAgAGYAcgBhAGMAXwBwAGEAcgB0ACwAIABBAEIAUwAoAGYAcgBhAGMAXwBwAGEAcgB0ACkAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABSAE8ATwBUADoAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeAAtAHQAaAAgAHIAbwBvAHQAIABvAGYAIABhACAAbgB1AG0AYgBlAHIAIAAoAG8AcgAgAHMAcQB1AGEAcgBlACAAcgBvAG8AdAAgAGkAZgAgAG4AbwAgAGQAZQBnAHIAZQBlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQAKQAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAcgBlAGEAbAAgAGQAZQBjAGkAbQBhAGwAIABuAHUAbQBiAGUAcgAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIAByAG8AbwB0ACAAbwBmACAAYABuAGAALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAG4AIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABUAGgAZQAgAG4AdQBtAGIAZQByACAAdABvACAAdABhAGsAZQAgAHQAaABlACAAcgBvAG8AdAAgAG8AZgAuAFwAbgAgACAAIAAtACAAeAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAFQAaABlACAAcgBvAG8AdAAgAGQAZQBnAHIAZQBlAC4AIABEAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAyACAAKABzAHEAdQBhAHIAZQAgAHIAbwBvAHQAKQAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABSAGUAagBlAGMAdABzACAAYQBsAGwAIABuAGUAZwBhAHQAaQB2AGUAIABpAG4AcAB1AHQAIAB2AGEAbAB1AGUAcwAgAGYAbwByACAAYABuAGAALAAgAHIAZQBnAGEAcgBkAGwAZQBzAHMAIABvAGYAIAByAG8AbwB0AC4AXABuACAAIAAgAC0AIABNAGkAbQBpAGMAcwAgAEUAeABjAGUAbAAnAHMAIABiAGUAaABhAHYAaQBvAHIAIAAoAHIAZQB0AHUAcgBuAHMAIAAjAE4AVQBNACEAIABpAGYAIAByAG8AbwB0ACAAdwBvAHUAbABkACAAYgBlACAAYwBvAG0AcABsAGUAeAApAC4AXABuACAAIAAgAC0AIABVAHMAZQAgAEUAeABjAGUAbAAZIHMAIABgAEkATQBQAE8AVwBFAFIAYAAgAG8AcgAgAGAASQBNAFMAUQBSAFQAYAAgAGYAbwByACAAYwBvAG0AcABsAGUAeAAgAG4AdQBtAGIAZQByACAAcwB1AHAAcABvAHIAdAAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgAFIATwBPAFQAKAAxADYAKQAgACAAIAAgACAAIAAgAJIhIAA0AFwAbgAgACAAIABSAE8ATwBUACgAMgA3ACwAIAAzACkAIAAgACAAIACSISAAMwBcAG4AIAAgACAAUgBPAE8AVAAoADkALAAgADAALgA1ACkAIAAgACAAkiEgADgAMQBcAG4AIAAgACAAUgBPAE8AVAAoAC0ANQAsACAAMwApACAAIAAgACAAkiEgACMATgBVAE0AIQBcAG4AKgAvAFwAbgBcAG4AUgBPAE8AVAAgAD0AIABMAEEATQBCAEQAQQAoAG4ALAAgAFsAeABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKAB4ACkALAAgADIALAAgAHgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAbgAgADwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMAUQBSAFQAKAAtADEAKQAsACAAIAAvAC8AIABUAHIAaQBnAGcAZQByAHMAIAAjAE4AVQBNACEAIABlAHIAcgBvAHIAIABmAG8AcgAgAG4AZQBnAGEAdABpAHYAZQAgAGIAYQBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AIABeACAAKAAxACAALwAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVABcAG4AIAAgACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAYQAgAG8AbgBlAC0AbABpAG4AZQAsACAAbABhAGIAZQBsAGUAZAAgAHYAZQByAHMAaQBvAG4AIABvAGYAIAB0AGgAZQAgAGYAbwByAG0AdQBsAGEAIABpAG4AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAGMAZQBsAGwALABcAG4AIAAgACAAbwBtAGkAdAB0AGkAbgBnACAAdABoAGUAIABsAGUAYQBkAGkAbgBnACAAZQBxAHUAYQBsACAAcwBpAGcAbgAgAGEAbgBkACAAcAByAGUAcABlAG4AZABpAG4AZwAgAHQAaABlACAAYwBlAGwAbAAgAHIAZQBmAGUAcgBlAG4AYwBlAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABjAGUAbABsACkAXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgACAAIABjAGUAbABsACAAOgAgAEEAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAbwAgAGEAIABjAGUAbABsACAAYwBvAG4AdABhAGkAbgBpAG4AZwAgAGEAIABmAG8AcgBtAHUAbABhAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgACAAIABBACAAcwBpAG4AZwBsAGUALQBsAGkAbgBlACAAcwB0AHIAaQBuAGcAIABpAG4AIAB0AGgAZQAgAGYAbwByAG0AYQB0ACAAXAAiAEEAMQA6AD0AIABGAE8AUgBNAFUATABBACgALgAuAC4AKQBcACIAXABuACAAIAAgACAAIABVAHMAZQBmAHUAbAAgAGYAbwByACAAYQB1AGQAaQB0AGkAbgBnACwAIABkAG8AYwB1AG0AZQBuAHQAYQB0AGkAbwBuACwAIABkAGEAcwBoAGIAbwBhAHIAZABzACwAIABvAHIAIAB0AGUAYQBjAGgAaQBuAGcAIAB0AG8AbwBsAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABCADMAKQAgACAAkiEgAFwAIgBCADMAOgA9ACAAUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAEMANQApACAAIACSISAAXAAiAEMANQA6AD0AIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAzACkAXAAiAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAAVABoAGUAIAByAGUAcwB1AGwAdAAgAGkAcwAgAGUAcQB1AGkAdgBhAGwAZQBuAHQAIAB0AG8AOgAgAEMARQBMAEwAKABcACIAYQBkAGQAcgBlAHMAcwBcACIALAAgAGMAZQBsAGwAKQAgACYAIABcACIAOgA9ACAAXAAiACAAJgAgAFQARQBYAFQAQQBGAFQARQBSACgARgBPAFIATQBVAEwAQQBUAEUAWABUACgAYwBlAGwAbAApACwAIABcACIAPQBcACIAKQBcAG4AIAAgACAAIAAgAC0AIABJAGYAIAB0AGgAZQAgAHIAZQBmAGUAcgBlAG4AYwBlAGQAIABjAGUAbABsACAAZABvAGUAcwAgAG4AbwB0ACAAYwBvAG4AdABhAGkAbgAgAGEAIABmAG8AcgBtAHUAbABhACwAIABhAG4AIABlAHIAcgBvAHIAIAB3AGkAbABsACAAbwBjAGMAdQByAC4AXABuACAAIAAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAGQAbwBlAHMAIABuAG8AdAAgAGUAdgBhAGwAdQBhAHQAZQAgAG8AcgAgAGEAbAB0AGUAcgAgAHQAaABlACAAZgBvAHIAbQB1AGwAYQAUIG8AbgBsAHkAIABmAG8AcgBtAGEAdABzACAAaQB0ACAAZgBvAHIAIABkAGkAcwBwAGwAYQB5AC4AXABuACoALwBcAG4AXABuAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUAD0ATABBAE0AQgBEAEEAKABcAG4AIAAgAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACwAIAAgAC8ALwAgAEEAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAbwAgAGEAIABjAGUAbABsACAAYwBvAG4AdABhAGkAbgBpAG4AZwAgAGEAIABmAG8AcgBtAHUAbABhAFwAbgBcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAAcgBhAHcALAAgAEYATwBSAE0AVQBMAEEAVABFAFgAVAAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABcACIAPQBSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIABjAGwAZQBhAG4ALAAgAFQARQBYAFQAQQBGAFQARQBSACgAcgBhAHcALAAgAFwAIgA9AFwAIgApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABcACIAUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAbABhAGIAZQBsACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAZgBvAHIAbQB1AGwAYQBfAGMAZQBsAGwAKQAsACAAXAAiACQAXAAiACwAIABcACIAXAAiACkAIAAmACAAXAAiADoAPQAgAFwAIgAsAFwAbgAgACAAIAAgAGwAYQBiAGUAbAAgACYAIABjAGwAZQBhAG4AXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUgBPAFUATgBEAF8ARgBJAFgAXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAgACAAUgBvAHUAbgBkAHMAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAcwAgAGEAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGEAIABzAHAAZQBjAGkAZgBpAGUAZAAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AXABuACAAIAAgAE8AcAB0AGkAbwBuAGEAbABsAHkAIAByAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAcwB1AGwAdAAgAGEAcwAgAGEAIABmAGkAeABlAGQALQB3AGkAZAB0AGgAIAB0AGUAeAB0ACAAcwB0AHIAaQBuAGcALAAgAHAAcgBlAHMAZQByAHYAaQBuAGcAIAB0AHIAYQBpAGwAaQBuAGcAIAB6AGUAcgBvAHMALgBcAG4AXABuACAAIAAgAFMAeQBuAHQAYQB4ADoAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAG4AdQBtAGIAZQByACwAIABwAGwAYQBjAGUAcwAsACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAbgB1AG0AYgBlAHIAIAAgACAAIAAgACAAOgAgAFQAaABlACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQAgAHQAbwAgAHAAcgBvAGMAZQBzAHMALgBcAG4AIAAgACAAIAAgAHAAbABhAGMAZQBzACAAIAAgACAAIAAgADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAZQB0AGEAaQBuAC4AXABuACAAIAAgACAAIABhAHMAXwB0AGUAeAB0ACAAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgBzACAAbwB1AHQAcAB1AHQAIABhAHMAIAB0AGUAeAB0ACAAKABlAC4AZwAuACwAIABcACIAMwAuADEANAAwAFwAIgApAC4AXABuACAAIAAgACAAIAB1AHMAZQBfAHIAbwB1AG4AZAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIABhAHAAcABsAGkAZQBzACAAcgBvAHUAbgBkAGkAbgBnAC4AIABPAHQAaABlAHIAdwBpAHMAZQAsACAAdAByAHUAbgBjAGEAdABlAHMALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIABuAHUAbQBiAGUAcgAgAG8AcgAgAHQAZQB4AHQAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIAByAG8AdQBuAGQAZQBkACAAbwByACAAdAByAHUAbgBjAGEAdABlAGQAIAB2AGEAbAB1AGUAIAB0AG8AIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAyACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgADMALgAxADQAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADMALAAgAFQAUgBVAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQBcACIAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADQALAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQApACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQA1AFwAIgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABGAEEATABTAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIAAzAC4AMQA0ADEANQA5ADIANgA1ADQAIAAgACAAKABjAGEAcABwAGUAZAAgAHQAbwAgADkAIABkAGUAYwBpAG0AYQBsAHMAKQBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABUAFIAVQBFACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxADUAOQAyADYANQAzADUAOQAwAFwAIgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAgACAALQAgAEUAeABjAGUAbAAgAGwAaQBtAGkAdABzACAAbgB1AG0AZQByAGkAYwAgAGQAaQBzAHAAbABhAHkAIABwAHIAZQBjAGkAcwBpAG8AbgAgAHQAbwAgAH4AOQAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuACAAVwBoAGUAbgAgAGEAcwBfAHQAZQB4AHQAIAA9ACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAIABpAHMAIABjAGEAcABwAGUAZAAgAGEAdAAgADkAIABkAGkAZwBpAHQAcwAgAGYAbwByACAAYwBvAG4AcwBpAHMAdABlAG4AYwB5AC4AXABuACAAIAAgACAAIAAtACAAVABvACAAZABpAHMAcABsAGEAeQAgAGYAdQBsAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgAG8AcgAgAHAAcgBlAHMAZQByAHYAZQAgAHQAcgBhAGkAbABpAG4AZwAgAHoAZQByAG8AcwAsACAAcwBlAHQAIABhAHMAXwB0AGUAeAB0ACAAPQAgAFQAUgBVAEUALgBcAG4AIAAgACAAIAAgAC0AIABTAHUAcABwAG8AcgB0AHMAIABiAG8AdABoACAAcgBvAHUAbgBkAGkAbgBnACAAYQBuAGQAIAB0AHIAdQBuAGMAYQB0AGkAbwBuACAAbQBvAGQAZQBzAC4AXABuACAAIAAgACAAIAAtACAASQBkAGUAYQBsACAAZgBvAHIAIABmAG8AcgBtAGEAdAB0AGkAbgBnACAAYwBvAG4AcwB0AGEAbgB0AHMALAAgAHYAaQBzAHUAYQBsACAAZABpAHMAcABsAGEAeQAgAGMAbwBuAHQAcgBvAGwALAAgAG8AcgAgAGUAbgBzAHUAcgBpAG4AZwAgAGMAbABlAGEAbgAgAG8AdQB0AHAAdQB0AHMAIABpAG4AIAByAGUAcABvAHIAdABzAC4AXABuACoALwBcAG4AXABuAFwAbgBSAE8AVQBOAEQAXwBGAEkAWAA9AEwAQQBNAEIARABBACgAXABuACAAIABuAHUAbQBiAGUAcgAsACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAZQBxAHUAaQByAGUAZAA6ACAAdABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAHIAbwB1AG4AZAAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAZQBcAG4AIAAgAHAAbABhAGMAZQBzACwAIAAgACAAIAAgACAAIAAgACAALwAvACAAUgBlAHEAdQBpAHIAZQBkADoAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAZQB0AGEAaQBuAFwAbgAgACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAOgAgAGkAZgAgAFQAUgBVAEUALAAgAHIAZQB0AHUAcgBuACAAcgBlAHMAdQBsAHQAIABhAHMAIAB0AGUAeAB0ACAAdwBpAHQAaAAgAGYAaQB4AGUAZAAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwBcAG4AIAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQAsACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAG8AdQBuAGQAOwAgAGkAZgAgAEYAQQBMAFMARQAgAG8AcgAgAG8AbQBpAHQAdABlAGQALAAgAHQAcgB1AG4AYwBhAHQAZQBcAG4AXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAG4ALAAgAE4AKABuAHUAbQBiAGUAcgApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARQBuAHMAdQByAGUAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0AFwAbgAgACAAIAAgAHIAYQB3AF8AcAAsACAATgAoAHAAbABhAGMAZQBzACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAYQB3ACAAaQBuAHAAdQB0ACAAZgBvAHIAIABwAGwAYQBjAGUAcwBcAG4AIAAgACAAIAByAG8AdQBuAGQAXwBmAGwAYQBnACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAdQBzAGUAXwByAG8AdQBuAGQAKQAsACAARgBBAEwAUwBFACwAIAB1AHMAZQBfAHIAbwB1AG4AZAApACwAXABuACAAIAAgACAAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAYQBzAF8AdABlAHgAdAApACwAIABGAEEATABTAEUALAAgAGEAcwBfAHQAZQB4AHQAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABFAHgAYwBlAGwAIABvAG4AbAB5ACAAcgBlAGwAaQBhAGIAbAB5ACAAZABpAHMAcABsAGEAeQBzACAAdQBwACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwAgAGEAcwAgAG4AdQBtAGUAcgBpAGMAXABuACAAIAAgACAAbQBhAHgAXwBwAGwAYQBjAGUAcwAsACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIAByAGEAdwBfAHAALAAgAE0ASQBOACgAcgBhAHcAXwBwACwAIAA5ACkAKQAsAFwAbgBcAG4AIAAgACAAIABwAHcAcgBfADEAMAAsACAAMQAwACAAXgAgAG0AYQB4AF8AcABsAGEAYwBlAHMALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFAAbwB3AGUAcgAgAG8AZgAgADEAMAAgAGYAbwByACAAcgBvAHUAbgBkAGkAbgBnAC8AdAByAHUAbgBjAGEAdABpAG8AbgBcAG4AXABuACAAIAAgACAALwAvACAAUABlAHIAZgBvAHIAbQAgAHIAbwB1AG4AZABpAG4AZwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAASQBGACgAcgBvAHUAbgBkAF8AZgBsAGEAZwAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAbgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACwAXABuACAAIAAgACAAIAAgACAAIABUAFIAVQBOAEMAKABuACAAKgAgAHAAdwByAF8AMQAwACkAIAAvACAAcAB3AHIAXwAxADAAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAGYAbwByAG0AYQB0ACAAYQBzACAAZgBpAHgAZQBkAC0AbABlAG4AZwB0AGgAIABzAHQAcgBpAG4AZwBcAG4AIAAgACAAIABmAGkAbgBhAGwALABcAG4AIAAgACAAIAAgACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAcgBlAHMAdQBsAHQALAAgAFwAIgAwAC4AXAAiACAAJgAgAFIARQBQAFQAKABcACIAMABcACIALAAgAG0AYQB4AF8AcABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABmAGkAbgBhAGwAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBSAEUAQwBJAFAAIgAsACIARgBSAEEAQwAiACwAIgBSAE8ATwBUACIALAAiAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACIALAAiAFIATwBVAE4ARABfAEYASQBYACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIATQBEAFkAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABSAEUAQwBJAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAYwBpAHAAcgBvAGMAYQBsACAAKABtAHUAbAB0AGkAcABsAGkAYwBhAHQAaQB2AGUAIABpAG4AdgBlAHIAcwBlACkAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAaQBuAGcAbABlACAAZABlAGMAaQBtAGEAbAAgAHYAYQBsAHUAZQAgAGUAcQB1AGEAbAAgAHQAbwAgADEAIABkAGkAdgBpAGQAZQBkACAAYgB5ACAAdABoAGUAIABpAG4AcAB1AHQALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAbgB5ACAAbgBvAG4AegBlAHIAbwAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAHQAdQByAG4AcwAgAGAAIwBEAEkAVgAvADAAIQBgACAAaQBmACAAaQBuAHAAdQB0ACAAaQBzACAAegBlAHIAbwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGYAbABpAHAAcABpAG4AZwAgAGYAcgBhAGMAdABpAG8AbgBzACwAIABjAG8AbgB2AGUAcgB0AGkAbgBnACAAcgBhAHQAZQBzACAAKABlAC4AZwAuACwAIABIAHoAIACUISAAcwBlAGMAbwBuAGQAcwApACwAIABvAHIAIABpAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGkAbwBzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAA0ACkAIACSISAAMAAuADIANQBcAG4AIAAgACAAIAAgAFIARQBDAEkAUAAoADAALgAyACkAIACSISAANQBcAG4AKgAvAFwAbgBSAEUAQwBJAFAAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgADEAIAAvACAAaQBuAHAAdQB0ACkAOwBcAG4AXABuAC8AKgAgAEYAUgBBAEMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAKABuAG8AbgAtAGkAbgB0AGUAZwBlAHIAKQAgAHAAYQByAHQAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAYwBhAGwAYQByACAAZABlAGMAaQBtAGEAbAAgAGIAZQB0AHcAZQBlAG4AIAAwACAAYQBuAGQAIAAxACAAKABvAHIAIAAtADEAIABhAG4AZAAgADAAIABpAGYAIABzAGkAZwBuACAAaQBzACAAcAByAGUAcwBlAHIAdgBlAGQAKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGUAeAB0AHIAYQBjAHQAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0ACAAZgByAG8AbQAuAFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAbQBvAGQAZQAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAwACkAXABuACAAIAAgACAAIAAgACAALQAgADAAOgAgAEEAbAB3AGEAeQBzACAAcgBlAHQAdQByAG4AIABwAG8AcwBpAHQAaQB2AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdABcAG4AIAAgACAAIAAgACAAIAAtACAAMQA6ACAAUAByAGUAcwBlAHIAdgBlACAAcwBpAGcAbgAgAG8AZgAgAGkAbgBwAHUAdAAgACgAZQAuAGcALgAsACAALQAzAC4AMgA1ACAAkiEgAC0AMAAuADIANQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABDAG8AbQBwAGwAZQBtAGUAbgB0AHMAIABFAHgAYwBlAGwAGSBzACAAVABSAFUATgBDACAAYQBuAGQAIABRAFUATwBUAEkARQBOAFQAIABmAHUAbgBjAHQAaQBvAG4AcwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGQAZQB0AGUAYwB0AGkAbgBnACAAZABlAGMAaQBtAGEAbAAgAHIAZQBtAGEAaQBuAGQAZQByAHMAIABhAG4AZAAgAGEAbgBhAGwAeQB6AGkAbgBnACAAbwBmAGYAcwBlAHQAcwAgAGYAcgBvAG0AIAB3AGgAbwBsAGUAIAB2AGEAbAB1AGUAcwAuAFwAbgAgACAAIAAtACAAUwBpAGcAbgAtAHAAcgBlAHMAZQByAHYAaQBuAGcAIABtAG8AZABlACAAYwBhAG4AIABpAG4AZABpAGMAYQB0AGUAIAB3AGgAZQB0AGgAZQByACAAYQAgAHYAYQBsAHUAZQAgAGkAcwAgAGoAdQBzAHQAIABhAGIAbwB2AGUAIABvAHIAIABqAHUAcwB0ACAAYgBlAGwAbwB3ACAAYQBuACAAaQBuAHQAZQBnAGUAcgAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgAEYAUgBBAEMAKAAtADMALgAyADUAKQAgACAAIAAgACAAIAAgAJIhIAAwAC4AMgA1ACAAIABcAG4AIAAgACAARgBSAEEAQwAoAC0AMwAuADIANQAsACAAMQApACAAIAAgACAAkiEgAC0AMAAuADIANQBcAG4AKgAvAFwAbgBGAFIAQQBDACAAPQAgAEwAQQBNAEIARABBACgAaQBuAHAAdQB0ACwAIABbAG0AbwBkAGUAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABEAGUAZgBhAHUAbAB0ACAAbQBvAGQAZQAgAHQAbwAgADAAIABpAGYAIABvAG0AaQB0AHQAZQBkACAAbwByACAAaQBuAHYAYQBsAGkAZABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALAAgAEkARgAoAE8AUgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABtAG8AZABlACAAPgAgADEAKQAsACAAMAAsACAAbQBvAGQAZQApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGIAeQAgAHMAdQBiAHQAcgBhAGMAdABpAG4AZwAgAGkAbgB0AGUAZwBlAHIAIABwAG8AcgB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAAZgByAGEAYwBfAHAAYQByAHQALAAgAGkAbgBwAHUAdAAgAC0AIABUAFIAVQBOAEMAKABpAG4AcAB1AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABSAGUAdAB1AHIAbgAgAHMAaQBnAG4AZQBkACAAbwByACAAYQBiAHMAbwBsAHUAdABlACAAdgBhAGwAdQBlACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAbQBvAGQAZQAgAD0AIAAxACwAIABmAHIAYQBjAF8AcABhAHIAdAAsACAAQQBCAFMAKABmAHIAYQBjAF8AcABhAHIAdAApACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUgBPAE8AVAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHgALQB0AGgAIAByAG8AbwB0ACAAbwBmACAAYQAgAG4AdQBtAGIAZQByACAAKABvAHIAIABzAHEAdQBhAHIAZQAgAHIAbwBvAHQAIABpAGYAIABuAG8AIABkAGUAZwByAGUAZQAgAGkAcwAgAHMAcABlAGMAaQBmAGkAZQBkACkALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHIAZQBhAGwAIABkAGUAYwBpAG0AYQBsACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAcgBvAG8AdAAgAG8AZgAgAGAAbgBgAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABuACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAHQAYQBrAGUAIAB0AGgAZQAgAHIAbwBvAHQAIABvAGYALgBcAG4AIAAgACAALQAgAHgAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABUAGgAZQAgAHIAbwBvAHQAIABkAGUAZwByAGUAZQAuACAARABlAGYAYQB1AGwAdABzACAAdABvACAAMgAgACgAcwBxAHUAYQByAGUAIAByAG8AbwB0ACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAGoAZQBjAHQAcwAgAGEAbABsACAAbgBlAGcAYQB0AGkAdgBlACAAaQBuAHAAdQB0ACAAdgBhAGwAdQBlAHMAIABmAG8AcgAgAGAAbgBgACwAIAByAGUAZwBhAHIAZABsAGUAcwBzACAAbwBmACAAcgBvAG8AdAAuAFwAbgAgACAAIAAtACAATQBpAG0AaQBjAHMAIABFAHgAYwBlAGwAJwBzACAAYgBlAGgAYQB2AGkAbwByACAAKAByAGUAdAB1AHIAbgBzACAAIwBOAFUATQAhACAAaQBmACAAcgBvAG8AdAAgAHcAbwB1AGwAZAAgAGIAZQAgAGMAbwBtAHAAbABlAHgAKQAuAFwAbgAgACAAIAAtACAAVQBzAGUAIABFAHgAYwBlAGwAGSBzACAAYABJAE0AUABPAFcARQBSAGAAIABvAHIAIABgAEkATQBTAFEAUgBUAGAAIABmAG8AcgAgAGMAbwBtAHAAbABlAHgAIABuAHUAbQBiAGUAcgAgAHMAdQBwAHAAbwByAHQALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIABSAE8ATwBUACgAMQA2ACkAIAAgACAAIAAgACAAIACSISAANABcAG4AIAAgACAAUgBPAE8AVAAoADIANwAsACAAMwApACAAIAAgACAAkiEgADMAXABuACAAIAAgAFIATwBPAFQAKAA5ACwAIAAwAC4ANQApACAAIAAgAJIhIAA4ADEAXABuACAAIAAgAFIATwBPAFQAKAAtADUALAAgADMAKQAgACAAIAAgAJIhIAAjAE4AVQBNACEAXABuACoALwBcAG4AUgBPAE8AVAAgAD0AIABMAEEATQBCAEQAQQAoAG4ALAAgAFsAeABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKAB4ACkALAAgADIALAAgAHgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAFEAUgBUACgALQAxACkALAAgAC8ALwAgAFQAcgBpAGcAZwBlAHIAcwAgACMATgBVAE0AIQAgAGUAcgByAG8AcgAgAGYAbwByACAAbgBlAGcAYQB0AGkAdgBlACAAYgBhAHMAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbgAgAF4AIAAoADEAIAAvACAAcgBvAG8AdABfAGQAZQBnAHIAZQBlACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUAFwAbgAgACAAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbwBuAGUALQBsAGkAbgBlACwAIABsAGEAYgBlAGwAZQBkACAAdgBlAHIAcwBpAG8AbgAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQB1AGwAYQAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAYwBlAGwAbAAsAFwAbgAgACAAIABvAG0AaQB0AHQAaQBuAGcAIAB0AGgAZQAgAGwAZQBhAGQAaQBuAGcAIABlAHEAdQBhAGwAIABzAGkAZwBuACAAYQBuAGQAIABwAHIAZQBwAGUAbgBkAGkAbgBnACAAdABoAGUAIABjAGUAbABsACAAcgBlAGYAZQByAGUAbgBjAGUALgBcAG4AXABuACAAIAAgAFMAeQBuAHQAYQB4ADoAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAGMAZQBsAGwAKQBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAAIAAgAGMAZQBsAGwAIAA6ACAAQQAgAHIAZQBmAGUAcgBlAG4AYwBlACAAdABvACAAYQAgAGMAZQBsAGwAIABjAG8AbgB0AGEAaQBuAGkAbgBnACAAYQAgAGYAbwByAG0AdQBsAGEALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIABzAGkAbgBnAGwAZQAtAGwAaQBuAGUAIABzAHQAcgBpAG4AZwAgAGkAbgAgAHQAaABlACAAZgBvAHIAbQBhAHQAIABcACIAQQAxADoAPQAgAEYATwBSAE0AVQBMAEEAKAAuAC4ALgApAFwAIgBcAG4AIAAgACAAIAAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABhAHUAZABpAHQAaQBuAGcALAAgAGQAbwBjAHUAbQBlAG4AdABhAHQAaQBvAG4ALAAgAGQAYQBzAGgAYgBvAGEAcgBkAHMALAAgAG8AcgAgAHQAZQBhAGMAaABpAG4AZwAgAHQAbwBvAGwAcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAEIAMwApACAAIACSISAAXAAiAEIAMwA6AD0AIABSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIAAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACgAQwA1ACkAIAAgAJIhIABcACIAQwA1ADoAPQAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsADMAKQBcACIAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAAIAAgAC0AIABUAGgAZQAgAHIAZQBzAHUAbAB0ACAAaQBzACAAZQBxAHUAaQB2AGEAbABlAG4AdAAgAHQAbwA6ACAAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAYwBlAGwAbAApACAAJgAgAFwAIgA6AD0AIABcACIAIAAmACAAVABFAFgAVABBAEYAVABFAFIAKABGAE8AUgBNAFUATABBAFQARQBYAFQAKABjAGUAbABsACkALAAgAFwAIgA9AFwAIgApAFwAbgAgACAAIAAgACAALQAgAEkAZgAgAHQAaABlACAAcgBlAGYAZQByAGUAbgBjAGUAZAAgAGMAZQBsAGwAIABkAG8AZQBzACAAbgBvAHQAIABjAG8AbgB0AGEAaQBuACAAYQAgAGYAbwByAG0AdQBsAGEALAAgAGEAbgAgAGUAcgByAG8AcgAgAHcAaQBsAGwAIABvAGMAYwB1AHIALgBcAG4AIAAgACAAIAAgAC0AIABUAGgAaQBzACAAZgB1AG4AYwB0AGkAbwBuACAAZABvAGUAcwAgAG4AbwB0ACAAZQB2AGEAbAB1AGEAdABlACAAbwByACAAYQBsAHQAZQByACAAdABoAGUAIABmAG8AcgBtAHUAbABhABQgbwBuAGwAeQAgAGYAbwByAG0AYQB0AHMAIABpAHQAIABmAG8AcgAgAGQAaQBzAHAAbABhAHkALgBcAG4AKgAvAFwAbgBGAE8AUgBNAFUATABBAF8AVABFAFgAVAAgAD0AIABMAEEATQBCAEQAQQAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACwAIAAvAC8AIABBACAAcgBlAGYAZQByAGUAbgBjAGUAIAB0AG8AIABhACAAYwBlAGwAbAAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABhACAAZgBvAHIAbQB1AGwAYQBcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcALAAgAEYATwBSAE0AVQBMAEEAVABFAFgAVAAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgAC8ALwAgAFwAIgA9AFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAYwBsAGUAYQBuACwAIABUAEUAWABUAEEARgBUAEUAUgAoAHIAYQB3ACwAIABcACIAPQBcACIAKQAsACAALwAvACAAXAAiAFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAZgBvAHIAbQB1AGwAYQBfAGMAZQBsAGwAKQAsACAAXAAiACQAXAAiACwAIABcACIAXAAiACkAIAAmACAAXAAiADoAPQAgAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsACAAJgAgAGMAbABlAGEAbgBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABSAE8AVQBOAEQAXwBGAEkAWABcAG4AIAAgACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABSAG8AdQBuAGQAcwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAZQBzACAAYQAgAG4AdQBtAGIAZQByACAAdABvACAAYQAgAHMAcABlAGMAaQBmAGkAZQBkACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgBcAG4AIAAgACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAHIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHIAZQBzAHUAbAB0ACAAYQBzACAAYQAgAGYAaQB4AGUAZAAtAHcAaQBkAHQAaAAgAHQAZQB4AHQAIABzAHQAcgBpAG4AZwAsACAAcAByAGUAcwBlAHIAdgBpAG4AZwAgAHQAcgBhAGkAbABpAG4AZwAgAHoAZQByAG8AcwAuAFwAbgBcAG4AIAAgACAAUwB5AG4AdABhAHgAOgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAbgB1AG0AYgBlAHIALAAgAHAAbABhAGMAZQBzACwAIABbAGEAcwBfAHQAZQB4AHQAXQAsACAAWwB1AHMAZQBfAHIAbwB1AG4AZABdACkAXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgACAAIABuAHUAbQBiAGUAcgAgACAAIAAgACAAIAA6ACAAVABoAGUAIABuAHUAbQBlAHIAaQBjACAAdgBhAGwAdQBlACAAdABvACAAcAByAG8AYwBlAHMAcwAuAFwAbgAgACAAIAAgACAAcABsAGEAYwBlAHMAIAAgACAAIAAgACAAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAdABvACAAcgBlAHQAYQBpAG4ALgBcAG4AIAAgACAAIAAgAGEAcwBfAHQAZQB4AHQAIAAgACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAARgBBAEwAUwBFACkALgAgAEkAZgAgAFQAUgBVAEUALAAgAHIAZQB0AHUAcgBuAHMAIABvAHUAdABwAHUAdAAgAGEAcwAgAHQAZQB4AHQAIAAoAGUALgBnAC4ALAAgAFwAIgAzAC4AMQA0ADAAXAAiACkALgBcAG4AIAAgACAAIAAgAHUAcwBlAF8AcgBvAHUAbgBkACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAARgBBAEwAUwBFACkALgAgAEkAZgAgAFQAUgBVAEUALAAgAGEAcABwAGwAaQBlAHMAIAByAG8AdQBuAGQAaQBuAGcALgAgAE8AdABoAGUAcgB3AGkAcwBlACwAIAB0AHIAdQBuAGMAYQB0AGUAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAgACAAQQAgAG4AdQBtAGIAZQByACAAbwByACAAdABlAHgAdAAgAHMAdAByAGkAbgBnACAAcgBlAHAAcgBlAHMAZQBuAHQAaQBuAGcAIAB0AGgAZQAgAHIAbwB1AG4AZABlAGQAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAZAAgAHYAYQBsAHUAZQAgAHQAbwAgAGYAaQB4AGUAZAAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADIAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAMwAuADEANABcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMwAsACAAVABSAFUARQApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxAFwAIgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAANAAsACAAVABSAFUARQAsACAARgBBAEwAUwBFACkAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxADUAXAAiAFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAxADIALAAgAEYAQQBMAFMARQApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgADMALgAxADQAMQA1ADkAMgA2ADUANAAgACAAIAAoAGMAYQBwAHAAZQBkACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwApAFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAxADIALAAgAFQAUgBVAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgAFwAIgAzAC4AMQA0ADEANQA5ADIANgA1ADMANQA5ADAAXAAiAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAARQB4AGMAZQBsACAAbABpAG0AaQB0AHMAIABuAHUAbQBlAHIAaQBjACAAZABpAHMAcABsAGEAeQAgAHAAcgBlAGMAaQBzAGkAbwBuACAAdABvACAAfgA5ACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AIABXAGgAZQBuACAAYQBzAF8AdABlAHgAdAAgAD0AIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAgAGkAcwAgAGMAYQBwAHAAZQBkACAAYQB0ACAAOQAgAGQAaQBnAGkAdABzACAAZgBvAHIAIABjAG8AbgBzAGkAcwB0AGUAbgBjAHkALgBcAG4AIAAgACAAIAAgAC0AIABUAG8AIABkAGkAcwBwAGwAYQB5ACAAZgB1AGwAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbwByACAAcAByAGUAcwBlAHIAdgBlACAAdAByAGEAaQBsAGkAbgBnACAAegBlAHIAbwBzACwAIABzAGUAdAAgAGEAcwBfAHQAZQB4AHQAIAA9ACAAVABSAFUARQAuAFwAbgAgACAAIAAgACAALQAgAFMAdQBwAHAAbwByAHQAcwAgAGIAbwB0AGgAIAByAG8AdQBuAGQAaQBuAGcAIABhAG4AZAAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AIABtAG8AZABlAHMALgBcAG4AIAAgACAAIAAgAC0AIABJAGQAZQBhAGwAIABmAG8AcgAgAGYAbwByAG0AYQB0AHQAaQBuAGcAIABjAG8AbgBzAHQAYQBuAHQAcwAsACAAdgBpAHMAdQBhAGwAIABkAGkAcwBwAGwAYQB5ACAAYwBvAG4AdAByAG8AbAAsACAAbwByACAAZQBuAHMAdQByAGkAbgBnACAAYwBsAGUAYQBuACAAbwB1AHQAcAB1AHQAcwAgAGkAbgAgAHIAZQBwAG8AcgB0AHMALgBcAG4AKgAvAFwAbgBSAE8AVQBOAEQAXwBGAEkAWAAgAD0AIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgAG4AdQBtAGIAZQByACwAIAAvAC8AIABSAGUAcQB1AGkAcgBlAGQAOgAgAHQAaABlACAAbgB1AG0AYgBlAHIAIAB0AG8AIAByAG8AdQBuAGQAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAXABuACAAIAAgACAAcABsAGEAYwBlAHMALAAgAC8ALwAgAFIAZQBxAHUAaQByAGUAZAA6ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAGUAdABhAGkAbgBcAG4AIAAgACAAIABbAGEAcwBfAHQAZQB4AHQAXQAsACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgAgAHIAZQBzAHUAbAB0ACAAYQBzACAAdABlAHgAdAAgAHcAaQB0AGgAIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAXABuACAAIAAgACAAWwB1AHMAZQBfAHIAbwB1AG4AZABdACwAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAOgAgAGkAZgAgAFQAUgBVAEUALAAgAHIAbwB1AG4AZAA7ACAAaQBmACAARgBBAEwAUwBFACAAbwByACAAbwBtAGkAdAB0AGUAZAAsACAAdAByAHUAbgBjAGEAdABlAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABuACwAIABOACgAbgB1AG0AYgBlAHIAKQAsACAALwAvACAARQBuAHMAdQByAGUAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0AFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcAXwBwACwAIABOACgAcABsAGEAYwBlAHMAKQAsACAALwAvACAAUgBhAHcAIABpAG4AcAB1AHQAIABmAG8AcgAgAHAAbABhAGMAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAF8AZgBsAGEAZwAsACAASQBGACgASQBTAEIATABBAE4ASwAoAHUAcwBlAF8AcgBvAHUAbgBkACkALAAgAEYAQQBMAFMARQAsACAAdQBzAGUAXwByAG8AdQBuAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAYQBzAF8AdABlAHgAdAApACwAIABGAEEATABTAEUALAAgAGEAcwBfAHQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABFAHgAYwBlAGwAIABvAG4AbAB5ACAAcgBlAGwAaQBhAGIAbAB5ACAAZABpAHMAcABsAGEAeQBzACAAdQBwACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwAgAGEAcwAgAG4AdQBtAGUAcgBpAGMAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHAAbABhAGMAZQBzACwAIABJAEYAKAByAGUAdAB1AHIAbgBfAHQAZQB4AHQALAAgAHIAYQB3AF8AcAAsACAATQBJAE4AKAByAGEAdwBfAHAALAAgADkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABwAHcAcgBfADEAMAAsACAAMQAwACAAXgAgAG0AYQB4AF8AcABsAGEAYwBlAHMALAAgAC8ALwAgAFAAbwB3AGUAcgAgAG8AZgAgADEAMAAgAGYAbwByACAAcgBvAHUAbgBkAGkAbgBnAC8AdAByAHUAbgBjAGEAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAUABlAHIAZgBvAHIAbQAgAHIAbwB1AG4AZABpAG4AZwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAcgBvAHUAbgBkAF8AZgBsAGEAZwAsACAAUgBPAFUATgBEACgAbgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACwAIABUAFIAVQBOAEMAKABuACAAKgAgAHAAdwByAF8AMQAwACkAIAAvACAAcAB3AHIAXwAxADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAbAB5ACAAZgBvAHIAbQBhAHQAIABhAHMAIABmAGkAeABlAGQALQBsAGUAbgBnAHQAaAAgAHMAdAByAGkAbgBnAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsACwAIABJAEYAKAByAGUAdAB1AHIAbgBfAHQAZQB4AHQALAAgAFQARQBYAFQAKAByAGUAcwB1AGwAdAAsACAAXAAiADAALgBcACIAIAAmACAAUgBFAFAAVAAoAFwAIgAwAFwAIgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACkALAAgAHIAZQBzAHUAbAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAGYAaQBuAGEAbABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABDAE8AVQBOAFQAQQBfAFMAVABSAEkAQwBUAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAYwBvAHUAbgB0ACAAbwBmACAAbgBvAG4ALQBiAGwAYQBuAGsALAAgAG4AbwBuAC0AZQBtAHAAdAB5ACwAIABhAG4AZAAgAG4AbwBuAC0AdwBoAGkAdABlAHMAcABhAGMAZQAtAG8AbgBsAHkAIAB2AGEAbAB1AGUAcwAgAGYAcgBvAG0AIABhACAAcgBhAG4AZwBlAC4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAAwACAAaQBmACAAbgBvACAAbQBlAGEAbgBpAG4AZwBmAHUAbAAgAGMAbwBuAHQAZQBuAHQAIABlAHgAaQBzAHQAcwAuAFwAbgBcAG4AIAAgACAASQBuAHAAdQB0AHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgADoAIABBACAAdgBlAHIAdABpAGMAYQBsACAAbABpAHMAdAAgAG8AcgAgAGEAbgB5ACAAcwBpAG4AZwBsAGUALQBjAG8AbAB1AG0AbgAgAHIAYQBuAGcAZQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAEkAbgB0AGUAZwBlAHIAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAYwBlAGwAbABzACAAdABoAGEAdAAgAGMAbwBuAHQAYQBpAG4AIABtAGUAYQBuAGkAbgBnAGYAdQBsACAAYwBvAG4AdABlAG4AdAAgACgAaQBnAG4AbwByAGUAcwAgAFwAIgBcACIALAAgAFwAIgAgAFwAIgApAFwAbgBcAG4AIAAgACAAQgBlAGgAYQB2AGkAbwByADoAXABuACAAIAAgAC0AIABJAGYAIAB0AGgAZQAgAHIAYQBuAGcAZQAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABiAGwAYQBuAGsAcwAgAG8AcgAgAHcAaABpAHQAZQBzAHAAYQBjAGUALQBvAG4AbAB5ACAAYwBlAGwAbABzACAAkiEgAHIAZQB0AHUAcgBuAHMAIAAwAFwAbgAgACAAIAAtACAATwB0AGgAZQByAHcAaQBzAGUAIAByAGUAdAB1AHIAbgBzACAAQwBPAFUATgBUAEEAKABpAG4AcAB1AHQAKQBcAG4AIAAgACAALQAgAEEAcwBzAHUAbQBlAHMAIABpAG4AcAB1AHQAIABpAHMAIABhACAAcwB0AGEAdABpAGMAIABvAHIAIABzAHQAcgB1AGMAdAB1AHIAZQBkACAAcgBhAG4AZwBlACAAKABuAG8AdAAgAGQAeQBuAGEAbQBpAGMAIABzAHAAaQBsAGwAKQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAoAHsAXAAiAGEAcABwAGwAZQBcACIALAAgAFwAIgBcACIALAAgAFwAIgAgAFwAIgAsACAAXAAiAGcAcgBhAHAAZQBcACIAfQApACAAkiEgADIAXABuACoALwBcAG4AQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAASQBGACgAQwBPAFUATgBUAEkARgAoAGkAbgBwAHUAdAAsACAAXAAiACoAPwBcACIAKQAgAD0AIAAwACwAIAAwACwAIABDAE8AVQBOAFQAQQAoAGkAbgBwAHUAdAApACkAKQA7ACIAfQBdACwAIgBwAHIAbwBqAGUAYwB0AE4AYQBtAGUAcwAiADoAWwAiAFIARQBDAEkAUAAiACwAIgBGAFIAQQBDACIALAAiAFIATwBPAFQAIgAsACIARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAIgAsACIAUgBPAFUATgBEAF8ARgBJAFgAIgAsACIAQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAiAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAFkATQBEACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Committing before commencing Math and Geometry utilities
</commit_message>
<xml_diff>
--- a/General Utilities/General Utlities.xlsx
+++ b/General Utilities/General Utlities.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a47027c9c1b1b6a/Documents/GitHub/Lambda-Development/General Utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Lambda-Development\General Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{8FCE266A-C6E4-AF47-9DAC-B6B63284E2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FAEECE-20C2-49D5-BD46-97F1D688F373}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB948F8-5CCD-4024-B82F-3AA3BA053EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="2010" windowWidth="28185" windowHeight="14190" xr2:uid="{7A445647-2974-6942-9320-70750788AE91}"/>
+    <workbookView xWindow="465" yWindow="360" windowWidth="26370" windowHeight="14970" xr2:uid="{7A445647-2974-6942-9320-70750788AE91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="COUNTA_STRICT">_xlfn.LAMBDA(_xlpm.input, IF(COUNTIF(_xlpm.input, "*?") = 0, 0, COUNTA(_xlpm.input)))</definedName>
+    <definedName name="FORMAT_AS_LIST">_xlfn.LAMBDA(_xlpm.range,_xlop.format,_xlop.style,_xlop.sort,_xlop.mode, _xlfn.LET(_xlpm.style, IF(OR(_xlfn.ISOMITTED(_xlpm.style), _xlpm.style &gt; 1), 0, _xlpm.style), _xlpm.format, IF(OR(_xlfn.ISOMITTED(_xlpm.format), _xlpm.format &gt; 1), 0, _xlpm.format), _xlpm.mode, IF(OR(_xlfn.ISOMITTED(_xlpm.mode), _xlpm.mode &gt; 1), 0, _xlpm.mode), _xlpm.sort, IF(OR(_xlfn.ISOMITTED(_xlpm.sort), _xlpm.sort &gt; 1), 0, _xlpm.sort), _xlpm.separator, IF(_xlpm.format = 0, ", ", "; "), _xlpm.list, _xlfn.SWITCH(_xlpm.mode, 0, _xlfn.TOCOL(_xlpm.range, 3), 1, _xlfn.UNIQUE(_xlfn.TOCOL(_xlpm.range, 3))), _xlpm.sorted, _xlfn.SWITCH(_xlpm.sort, 0, _xlpm.list, 1, _xlfn._xlws.SORT(_xlpm.list)), _xlpm.output, _xlfn.SWITCH(_xlpm.style, 0, "{" &amp; _xlfn.TEXTJOIN(_xlpm.separator, , _xlpm.sorted) &amp; "}", 1, _xlfn.TEXTJOIN(_xlpm.separator, , _xlpm.sorted)), _xlpm.output))</definedName>
     <definedName name="FORMULA_TEXT">_xlfn.LAMBDA(_xlpm.formula_cell, _xlfn.LET(_xlpm.raw, _xlfn.FORMULATEXT(_xlpm.formula_cell), _xlpm.clean, _xlfn.TEXTAFTER(_xlpm.raw, "="), _xlpm.label, SUBSTITUTE(CELL("address", _xlpm.formula_cell), "$", "") &amp; ":= ", _xlpm.label &amp; _xlpm.clean))</definedName>
     <definedName name="FRAC">_xlfn.LAMBDA(_xlpm.input,_xlop.mode, _xlfn.LET(_xlpm.mode, IF(OR(_xlfn.ISOMITTED(_xlpm.mode), _xlpm.mode &gt; 1), 0, _xlpm.mode), _xlpm.frac_part, _xlpm.input - TRUNC(_xlpm.input), IF(_xlpm.mode = 1, _xlpm.frac_part, ABS(_xlpm.frac_part))))</definedName>
     <definedName name="RECIP">_xlfn.LAMBDA(_xlpm.input, 1 / _xlpm.input)</definedName>
@@ -435,7 +436,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="808" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -588,7 +589,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABSAEUAQwBJAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAYwBpAHAAcgBvAGMAYQBsACAAKABtAHUAbAB0AGkAcABsAGkAYwBhAHQAaQB2AGUAIABpAG4AdgBlAHIAcwBlACkAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAaQBuAGcAbABlACAAZABlAGMAaQBtAGEAbAAgAHYAYQBsAHUAZQAgAGUAcQB1AGEAbAAgAHQAbwAgADEAIABkAGkAdgBpAGQAZQBkACAAYgB5ACAAdABoAGUAIABpAG4AcAB1AHQALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAbgB5ACAAbgBvAG4AegBlAHIAbwAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAHQAdQByAG4AcwAgAGAAIwBEAEkAVgAvADAAIQBgACAAaQBmACAAaQBuAHAAdQB0ACAAaQBzACAAegBlAHIAbwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGYAbABpAHAAcABpAG4AZwAgAGYAcgBhAGMAdABpAG8AbgBzACwAIABjAG8AbgB2AGUAcgB0AGkAbgBnACAAcgBhAHQAZQBzACAAKABlAC4AZwAuACwAIABIAHoAIACUISAAcwBlAGMAbwBuAGQAcwApACwAIABvAHIAIABpAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGkAbwBzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAA0ACkAIACSISAAMAAuADIANQBcAG4AIAAgACAAIAAgAFIARQBDAEkAUAAoADAALgAyACkAIACSISAANQBcAG4AKgAvAFwAbgBSAEUAQwBJAFAAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgADEAIAAvACAAaQBuAHAAdQB0ACkAOwBcAG4AXABuAC8AKgAgAEYAUgBBAEMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAKABuAG8AbgAtAGkAbgB0AGUAZwBlAHIAKQAgAHAAYQByAHQAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAYwBhAGwAYQByACAAZABlAGMAaQBtAGEAbAAgAGIAZQB0AHcAZQBlAG4AIAAwACAAYQBuAGQAIAAxACAAKABvAHIAIAAtADEAIABhAG4AZAAgADAAIABpAGYAIABzAGkAZwBuACAAaQBzACAAcAByAGUAcwBlAHIAdgBlAGQAKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGUAeAB0AHIAYQBjAHQAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0ACAAZgByAG8AbQAuAFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAbQBvAGQAZQAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAwACkAXABuACAAIAAgACAAIAAgACAALQAgADAAOgAgAEEAbAB3AGEAeQBzACAAcgBlAHQAdQByAG4AIABwAG8AcwBpAHQAaQB2AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdABcAG4AIAAgACAAIAAgACAAIAAtACAAMQA6ACAAUAByAGUAcwBlAHIAdgBlACAAcwBpAGcAbgAgAG8AZgAgAGkAbgBwAHUAdAAgACgAZQAuAGcALgAsACAALQAzAC4AMgA1ACAAkiEgAC0AMAAuADIANQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABDAG8AbQBwAGwAZQBtAGUAbgB0AHMAIABFAHgAYwBlAGwAGSBzACAAVABSAFUATgBDACAAYQBuAGQAIABRAFUATwBUAEkARQBOAFQAIABmAHUAbgBjAHQAaQBvAG4AcwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGQAZQB0AGUAYwB0AGkAbgBnACAAZABlAGMAaQBtAGEAbAAgAHIAZQBtAGEAaQBuAGQAZQByAHMAIABhAG4AZAAgAGEAbgBhAGwAeQB6AGkAbgBnACAAbwBmAGYAcwBlAHQAcwAgAGYAcgBvAG0AIAB3AGgAbwBsAGUAIAB2AGEAbAB1AGUAcwAuAFwAbgAgACAAIAAtACAAUwBpAGcAbgAtAHAAcgBlAHMAZQByAHYAaQBuAGcAIABtAG8AZABlACAAYwBhAG4AIABpAG4AZABpAGMAYQB0AGUAIAB3AGgAZQB0AGgAZQByACAAYQAgAHYAYQBsAHUAZQAgAGkAcwAgAGoAdQBzAHQAIABhAGIAbwB2AGUAIABvAHIAIABqAHUAcwB0ACAAYgBlAGwAbwB3ACAAYQBuACAAaQBuAHQAZQBnAGUAcgAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgAEYAUgBBAEMAKAAtADMALgAyADUAKQAgACAAIAAgACAAIAAgAJIhIAAwAC4AMgA1ACAAIABcAG4AIAAgACAARgBSAEEAQwAoAC0AMwAuADIANQAsACAAMQApACAAIAAgACAAkiEgAC0AMAAuADIANQBcAG4AKgAvAFwAbgBGAFIAQQBDACAAPQAgAEwAQQBNAEIARABBACgAaQBuAHAAdQB0ACwAIABbAG0AbwBkAGUAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABEAGUAZgBhAHUAbAB0ACAAbQBvAGQAZQAgAHQAbwAgADAAIABpAGYAIABvAG0AaQB0AHQAZQBkACAAbwByACAAaQBuAHYAYQBsAGkAZABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALAAgAEkARgAoAE8AUgAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBvAGQAZQApACwAIABtAG8AZABlACAAPgAgADEAKQAsACAAMAAsACAAbQBvAGQAZQApACwAXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGIAeQAgAHMAdQBiAHQAcgBhAGMAdABpAG4AZwAgAGkAbgB0AGUAZwBlAHIAIABwAG8AcgB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAAZgByAGEAYwBfAHAAYQByAHQALAAgAGkAbgBwAHUAdAAgAC0AIABUAFIAVQBOAEMAKABpAG4AcAB1AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABSAGUAdAB1AHIAbgAgAHMAaQBnAG4AZQBkACAAbwByACAAYQBiAHMAbwBsAHUAdABlACAAdgBhAGwAdQBlACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAbQBvAGQAZQAgAD0AIAAxACwAIABmAHIAYQBjAF8AcABhAHIAdAAsACAAQQBCAFMAKABmAHIAYQBjAF8AcABhAHIAdAApACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUgBPAE8AVAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHgALQB0AGgAIAByAG8AbwB0ACAAbwBmACAAYQAgAG4AdQBtAGIAZQByACAAKABvAHIAIABzAHEAdQBhAHIAZQAgAHIAbwBvAHQAIABpAGYAIABuAG8AIABkAGUAZwByAGUAZQAgAGkAcwAgAHMAcABlAGMAaQBmAGkAZQBkACkALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHIAZQBhAGwAIABkAGUAYwBpAG0AYQBsACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAcgBvAG8AdAAgAG8AZgAgAGAAbgBgAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABuACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAHQAYQBrAGUAIAB0AGgAZQAgAHIAbwBvAHQAIABvAGYALgBcAG4AIAAgACAALQAgAHgAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABUAGgAZQAgAHIAbwBvAHQAIABkAGUAZwByAGUAZQAuACAARABlAGYAYQB1AGwAdABzACAAdABvACAAMgAgACgAcwBxAHUAYQByAGUAIAByAG8AbwB0ACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAGoAZQBjAHQAcwAgAGEAbABsACAAbgBlAGcAYQB0AGkAdgBlACAAaQBuAHAAdQB0ACAAdgBhAGwAdQBlAHMAIABmAG8AcgAgAGAAbgBgACwAIAByAGUAZwBhAHIAZABsAGUAcwBzACAAbwBmACAAcgBvAG8AdAAuAFwAbgAgACAAIAAtACAATQBpAG0AaQBjAHMAIABFAHgAYwBlAGwAJwBzACAAYgBlAGgAYQB2AGkAbwByACAAKAByAGUAdAB1AHIAbgBzACAAIwBOAFUATQAhACAAaQBmACAAcgBvAG8AdAAgAHcAbwB1AGwAZAAgAGIAZQAgAGMAbwBtAHAAbABlAHgAKQAuAFwAbgAgACAAIAAtACAAVQBzAGUAIABFAHgAYwBlAGwAGSBzACAAYABJAE0AUABPAFcARQBSAGAAIABvAHIAIABgAEkATQBTAFEAUgBUAGAAIABmAG8AcgAgAGMAbwBtAHAAbABlAHgAIABuAHUAbQBiAGUAcgAgAHMAdQBwAHAAbwByAHQALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIABSAE8ATwBUACgAMQA2ACkAIAAgACAAIAAgACAAIACSISAANABcAG4AIAAgACAAUgBPAE8AVAAoADIANwAsACAAMwApACAAIAAgACAAkiEgADMAXABuACAAIAAgAFIATwBPAFQAKAA5ACwAIAAwAC4ANQApACAAIAAgAJIhIAA4ADEAXABuACAAIAAgAFIATwBPAFQAKAAtADUALAAgADMAKQAgACAAIAAgAJIhIAAjAE4AVQBNACEAXABuACoALwBcAG4AUgBPAE8AVAAgAD0AIABMAEEATQBCAEQAQQAoAG4ALAAgAFsAeABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKAB4ACkALAAgADIALAAgAHgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAFEAUgBUACgALQAxACkALAAgAC8ALwAgAFQAcgBpAGcAZwBlAHIAcwAgACMATgBVAE0AIQAgAGUAcgByAG8AcgAgAGYAbwByACAAbgBlAGcAYQB0AGkAdgBlACAAYgBhAHMAZQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbgAgAF4AIAAoADEAIAAvACAAcgBvAG8AdABfAGQAZQBnAHIAZQBlACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUAFwAbgAgACAAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAbwBuAGUALQBsAGkAbgBlACwAIABsAGEAYgBlAGwAZQBkACAAdgBlAHIAcwBpAG8AbgAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQB1AGwAYQAgAGkAbgAgAHQAaABlACAAZwBpAHYAZQBuACAAYwBlAGwAbAAsAFwAbgAgACAAIABvAG0AaQB0AHQAaQBuAGcAIAB0AGgAZQAgAGwAZQBhAGQAaQBuAGcAIABlAHEAdQBhAGwAIABzAGkAZwBuACAAYQBuAGQAIABwAHIAZQBwAGUAbgBkAGkAbgBnACAAdABoAGUAIABjAGUAbABsACAAcgBlAGYAZQByAGUAbgBjAGUALgBcAG4AXABuACAAIAAgAFMAeQBuAHQAYQB4ADoAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAGMAZQBsAGwAKQBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAAIAAgAGMAZQBsAGwAIAA6ACAAQQAgAHIAZQBmAGUAcgBlAG4AYwBlACAAdABvACAAYQAgAGMAZQBsAGwAIABjAG8AbgB0AGEAaQBuAGkAbgBnACAAYQAgAGYAbwByAG0AdQBsAGEALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIABzAGkAbgBnAGwAZQAtAGwAaQBuAGUAIABzAHQAcgBpAG4AZwAgAGkAbgAgAHQAaABlACAAZgBvAHIAbQBhAHQAIABcACIAQQAxADoAPQAgAEYATwBSAE0AVQBMAEEAKAAuAC4ALgApAFwAIgBcAG4AIAAgACAAIAAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABhAHUAZABpAHQAaQBuAGcALAAgAGQAbwBjAHUAbQBlAG4AdABhAHQAaQBvAG4ALAAgAGQAYQBzAGgAYgBvAGEAcgBkAHMALAAgAG8AcgAgAHQAZQBhAGMAaABpAG4AZwAgAHQAbwBvAGwAcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAEIAMwApACAAIACSISAAXAAiAEIAMwA6AD0AIABSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIAAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACgAQwA1ACkAIAAgAJIhIABcACIAQwA1ADoAPQAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsADMAKQBcACIAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAAIAAgAC0AIABUAGgAZQAgAHIAZQBzAHUAbAB0ACAAaQBzACAAZQBxAHUAaQB2AGEAbABlAG4AdAAgAHQAbwA6ACAAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAYwBlAGwAbAApACAAJgAgAFwAIgA6AD0AIABcACIAIAAmACAAVABFAFgAVABBAEYAVABFAFIAKABGAE8AUgBNAFUATABBAFQARQBYAFQAKABjAGUAbABsACkALAAgAFwAIgA9AFwAIgApAFwAbgAgACAAIAAgACAALQAgAEkAZgAgAHQAaABlACAAcgBlAGYAZQByAGUAbgBjAGUAZAAgAGMAZQBsAGwAIABkAG8AZQBzACAAbgBvAHQAIABjAG8AbgB0AGEAaQBuACAAYQAgAGYAbwByAG0AdQBsAGEALAAgAGEAbgAgAGUAcgByAG8AcgAgAHcAaQBsAGwAIABvAGMAYwB1AHIALgBcAG4AIAAgACAAIAAgAC0AIABUAGgAaQBzACAAZgB1AG4AYwB0AGkAbwBuACAAZABvAGUAcwAgAG4AbwB0ACAAZQB2AGEAbAB1AGEAdABlACAAbwByACAAYQBsAHQAZQByACAAdABoAGUAIABmAG8AcgBtAHUAbABhABQgbwBuAGwAeQAgAGYAbwByAG0AYQB0AHMAIABpAHQAIABmAG8AcgAgAGQAaQBzAHAAbABhAHkALgBcAG4AKgAvAFwAbgBGAE8AUgBNAFUATABBAF8AVABFAFgAVAAgAD0AIABMAEEATQBCAEQAQQAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACwAIAAvAC8AIABBACAAcgBlAGYAZQByAGUAbgBjAGUAIAB0AG8AIABhACAAYwBlAGwAbAAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABhACAAZgBvAHIAbQB1AGwAYQBcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcALAAgAEYATwBSAE0AVQBMAEEAVABFAFgAVAAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgAC8ALwAgAFwAIgA9AFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAYwBsAGUAYQBuACwAIABUAEUAWABUAEEARgBUAEUAUgAoAHIAYQB3ACwAIABcACIAPQBcACIAKQAsACAALwAvACAAXAAiAFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAZgBvAHIAbQB1AGwAYQBfAGMAZQBsAGwAKQAsACAAXAAiACQAXAAiACwAIABcACIAXAAiACkAIAAmACAAXAAiADoAPQAgAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsACAAJgAgAGMAbABlAGEAbgBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABSAE8AVQBOAEQAXwBGAEkAWABcAG4AIAAgACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABSAG8AdQBuAGQAcwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAZQBzACAAYQAgAG4AdQBtAGIAZQByACAAdABvACAAYQAgAHMAcABlAGMAaQBmAGkAZQBkACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgBcAG4AIAAgACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAHIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHIAZQBzAHUAbAB0ACAAYQBzACAAYQAgAGYAaQB4AGUAZAAtAHcAaQBkAHQAaAAgAHQAZQB4AHQAIABzAHQAcgBpAG4AZwAsACAAcAByAGUAcwBlAHIAdgBpAG4AZwAgAHQAcgBhAGkAbABpAG4AZwAgAHoAZQByAG8AcwAuAFwAbgBcAG4AIAAgACAAUwB5AG4AdABhAHgAOgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAbgB1AG0AYgBlAHIALAAgAHAAbABhAGMAZQBzACwAIABbAGEAcwBfAHQAZQB4AHQAXQAsACAAWwB1AHMAZQBfAHIAbwB1AG4AZABdACkAXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgACAAIABuAHUAbQBiAGUAcgAgACAAIAAgACAAIAA6ACAAVABoAGUAIABuAHUAbQBlAHIAaQBjACAAdgBhAGwAdQBlACAAdABvACAAcAByAG8AYwBlAHMAcwAuAFwAbgAgACAAIAAgACAAcABsAGEAYwBlAHMAIAAgACAAIAAgACAAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAdABvACAAcgBlAHQAYQBpAG4ALgBcAG4AIAAgACAAIAAgAGEAcwBfAHQAZQB4AHQAIAAgACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAARgBBAEwAUwBFACkALgAgAEkAZgAgAFQAUgBVAEUALAAgAHIAZQB0AHUAcgBuAHMAIABvAHUAdABwAHUAdAAgAGEAcwAgAHQAZQB4AHQAIAAoAGUALgBnAC4ALAAgAFwAIgAzAC4AMQA0ADAAXAAiACkALgBcAG4AIAAgACAAIAAgAHUAcwBlAF8AcgBvAHUAbgBkACAAIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAARgBBAEwAUwBFACkALgAgAEkAZgAgAFQAUgBVAEUALAAgAGEAcABwAGwAaQBlAHMAIAByAG8AdQBuAGQAaQBuAGcALgAgAE8AdABoAGUAcgB3AGkAcwBlACwAIAB0AHIAdQBuAGMAYQB0AGUAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAgACAAQQAgAG4AdQBtAGIAZQByACAAbwByACAAdABlAHgAdAAgAHMAdAByAGkAbgBnACAAcgBlAHAAcgBlAHMAZQBuAHQAaQBuAGcAIAB0AGgAZQAgAHIAbwB1AG4AZABlAGQAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAZAAgAHYAYQBsAHUAZQAgAHQAbwAgAGYAaQB4AGUAZAAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADIAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAMwAuADEANABcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMwAsACAAVABSAFUARQApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxAFwAIgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAANAAsACAAVABSAFUARQAsACAARgBBAEwAUwBFACkAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxADUAXAAiAFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAxADIALAAgAEYAQQBMAFMARQApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgADMALgAxADQAMQA1ADkAMgA2ADUANAAgACAAIAAoAGMAYQBwAHAAZQBkACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwApAFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAxADIALAAgAFQAUgBVAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgAFwAIgAzAC4AMQA0ADEANQA5ADIANgA1ADMANQA5ADAAXAAiAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAARQB4AGMAZQBsACAAbABpAG0AaQB0AHMAIABuAHUAbQBlAHIAaQBjACAAZABpAHMAcABsAGEAeQAgAHAAcgBlAGMAaQBzAGkAbwBuACAAdABvACAAfgA5ACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AIABXAGgAZQBuACAAYQBzAF8AdABlAHgAdAAgAD0AIABGAEEATABTAEUALABcAG4AIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAgAGkAcwAgAGMAYQBwAHAAZQBkACAAYQB0ACAAOQAgAGQAaQBnAGkAdABzACAAZgBvAHIAIABjAG8AbgBzAGkAcwB0AGUAbgBjAHkALgBcAG4AIAAgACAAIAAgAC0AIABUAG8AIABkAGkAcwBwAGwAYQB5ACAAZgB1AGwAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAbwByACAAcAByAGUAcwBlAHIAdgBlACAAdAByAGEAaQBsAGkAbgBnACAAegBlAHIAbwBzACwAIABzAGUAdAAgAGEAcwBfAHQAZQB4AHQAIAA9ACAAVABSAFUARQAuAFwAbgAgACAAIAAgACAALQAgAFMAdQBwAHAAbwByAHQAcwAgAGIAbwB0AGgAIAByAG8AdQBuAGQAaQBuAGcAIABhAG4AZAAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AIABtAG8AZABlAHMALgBcAG4AIAAgACAAIAAgAC0AIABJAGQAZQBhAGwAIABmAG8AcgAgAGYAbwByAG0AYQB0AHQAaQBuAGcAIABjAG8AbgBzAHQAYQBuAHQAcwAsACAAdgBpAHMAdQBhAGwAIABkAGkAcwBwAGwAYQB5ACAAYwBvAG4AdAByAG8AbAAsACAAbwByACAAZQBuAHMAdQByAGkAbgBnACAAYwBsAGUAYQBuACAAbwB1AHQAcAB1AHQAcwAgAGkAbgAgAHIAZQBwAG8AcgB0AHMALgBcAG4AKgAvAFwAbgBSAE8AVQBOAEQAXwBGAEkAWAAgAD0AIABMAEEATQBCAEQAQQAoAFwAbgAgACAAIAAgAG4AdQBtAGIAZQByACwAIAAvAC8AIABSAGUAcQB1AGkAcgBlAGQAOgAgAHQAaABlACAAbgB1AG0AYgBlAHIAIAB0AG8AIAByAG8AdQBuAGQAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAXABuACAAIAAgACAAcABsAGEAYwBlAHMALAAgAC8ALwAgAFIAZQBxAHUAaQByAGUAZAA6ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAGUAdABhAGkAbgBcAG4AIAAgACAAIABbAGEAcwBfAHQAZQB4AHQAXQAsACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgAgAHIAZQBzAHUAbAB0ACAAYQBzACAAdABlAHgAdAAgAHcAaQB0AGgAIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAXABuACAAIAAgACAAWwB1AHMAZQBfAHIAbwB1AG4AZABdACwAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAOgAgAGkAZgAgAFQAUgBVAEUALAAgAHIAbwB1AG4AZAA7ACAAaQBmACAARgBBAEwAUwBFACAAbwByACAAbwBtAGkAdAB0AGUAZAAsACAAdAByAHUAbgBjAGEAdABlAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABuACwAIABOACgAbgB1AG0AYgBlAHIAKQAsACAALwAvACAARQBuAHMAdQByAGUAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0AFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcAXwBwACwAIABOACgAcABsAGEAYwBlAHMAKQAsACAALwAvACAAUgBhAHcAIABpAG4AcAB1AHQAIABmAG8AcgAgAHAAbABhAGMAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAF8AZgBsAGEAZwAsACAASQBGACgASQBTAEIATABBAE4ASwAoAHUAcwBlAF8AcgBvAHUAbgBkACkALAAgAEYAQQBMAFMARQAsACAAdQBzAGUAXwByAG8AdQBuAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAYQBzAF8AdABlAHgAdAApACwAIABGAEEATABTAEUALAAgAGEAcwBfAHQAZQB4AHQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABFAHgAYwBlAGwAIABvAG4AbAB5ACAAcgBlAGwAaQBhAGIAbAB5ACAAZABpAHMAcABsAGEAeQBzACAAdQBwACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwAgAGEAcwAgAG4AdQBtAGUAcgBpAGMAXABuACAAIAAgACAAIAAgACAAIABtAGEAeABfAHAAbABhAGMAZQBzACwAIABJAEYAKAByAGUAdAB1AHIAbgBfAHQAZQB4AHQALAAgAHIAYQB3AF8AcAAsACAATQBJAE4AKAByAGEAdwBfAHAALAAgADkAKQApACwAXABuACAAIAAgACAAIAAgACAAIABwAHcAcgBfADEAMAAsACAAMQAwACAAXgAgAG0AYQB4AF8AcABsAGEAYwBlAHMALAAgAC8ALwAgAFAAbwB3AGUAcgAgAG8AZgAgADEAMAAgAGYAbwByACAAcgBvAHUAbgBkAGkAbgBnAC8AdAByAHUAbgBjAGEAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAUABlAHIAZgBvAHIAbQAgAHIAbwB1AG4AZABpAG4AZwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAcgBvAHUAbgBkAF8AZgBsAGEAZwAsACAAUgBPAFUATgBEACgAbgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACwAIABUAFIAVQBOAEMAKABuACAAKgAgAHAAdwByAF8AMQAwACkAIAAvACAAcAB3AHIAXwAxADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAbAB5ACAAZgBvAHIAbQBhAHQAIABhAHMAIABmAGkAeABlAGQALQBsAGUAbgBnAHQAaAAgAHMAdAByAGkAbgBnAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsACwAIABJAEYAKAByAGUAdAB1AHIAbgBfAHQAZQB4AHQALAAgAFQARQBYAFQAKAByAGUAcwB1AGwAdAAsACAAXAAiADAALgBcACIAIAAmACAAUgBFAFAAVAAoAFwAIgAwAFwAIgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACkALAAgAHIAZQBzAHUAbAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAGYAaQBuAGEAbABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABDAE8AVQBOAFQAQQBfAFMAVABSAEkAQwBUAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIABhACAAYwBvAHUAbgB0ACAAbwBmACAAbgBvAG4ALQBiAGwAYQBuAGsALAAgAG4AbwBuAC0AZQBtAHAAdAB5ACwAIABhAG4AZAAgAG4AbwBuAC0AdwBoAGkAdABlAHMAcABhAGMAZQAtAG8AbgBsAHkAIAB2AGEAbAB1AGUAcwAgAGYAcgBvAG0AIABhACAAcgBhAG4AZwBlAC4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAAwACAAaQBmACAAbgBvACAAbQBlAGEAbgBpAG4AZwBmAHUAbAAgAGMAbwBuAHQAZQBuAHQAIABlAHgAaQBzAHQAcwAuAFwAbgBcAG4AIAAgACAASQBuAHAAdQB0AHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgADoAIABBACAAdgBlAHIAdABpAGMAYQBsACAAbABpAHMAdAAgAG8AcgAgAGEAbgB5ACAAcwBpAG4AZwBsAGUALQBjAG8AbAB1AG0AbgAgAHIAYQBuAGcAZQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAEkAbgB0AGUAZwBlAHIAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAYwBlAGwAbABzACAAdABoAGEAdAAgAGMAbwBuAHQAYQBpAG4AIABtAGUAYQBuAGkAbgBnAGYAdQBsACAAYwBvAG4AdABlAG4AdAAgACgAaQBnAG4AbwByAGUAcwAgAFwAIgBcACIALAAgAFwAIgAgAFwAIgApAFwAbgBcAG4AIAAgACAAQgBlAGgAYQB2AGkAbwByADoAXABuACAAIAAgAC0AIABJAGYAIAB0AGgAZQAgAHIAYQBuAGcAZQAgAGMAbwBuAHQAYQBpAG4AcwAgAG8AbgBsAHkAIABiAGwAYQBuAGsAcwAgAG8AcgAgAHcAaABpAHQAZQBzAHAAYQBjAGUALQBvAG4AbAB5ACAAYwBlAGwAbABzACAAkiEgAHIAZQB0AHUAcgBuAHMAIAAwAFwAbgAgACAAIAAtACAATwB0AGgAZQByAHcAaQBzAGUAIAByAGUAdAB1AHIAbgBzACAAQwBPAFUATgBUAEEAKABpAG4AcAB1AHQAKQBcAG4AIAAgACAALQAgAEEAcwBzAHUAbQBlAHMAIABpAG4AcAB1AHQAIABpAHMAIABhACAAcwB0AGEAdABpAGMAIABvAHIAIABzAHQAcgB1AGMAdAB1AHIAZQBkACAAcgBhAG4AZwBlACAAKABuAG8AdAAgAGQAeQBuAGEAbQBpAGMAIABzAHAAaQBsAGwAKQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAoAHsAXAAiAGEAcABwAGwAZQBcACIALAAgAFwAIgBcACIALAAgAFwAIgAgAFwAIgAsACAAXAAiAGcAcgBhAHAAZQBcACIAfQApACAAkiEgADIAXABuACoALwBcAG4AQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAASQBGACgAQwBPAFUATgBUAEkARgAoAGkAbgBwAHUAdAAsACAAXAAiACoAPwBcACIAKQAgAD0AIAAwACwAIAAwACwAIABDAE8AVQBOAFQAQQAoAGkAbgBwAHUAdAApACkAKQA7ACIAfQBdACwAIgBwAHIAbwBqAGUAYwB0AE4AYQBtAGUAcwAiADoAWwAiAFIARQBDAEkAUAAiACwAIgBGAFIAQQBDACIALAAiAFIATwBPAFQAIgAsACIARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAIgAsACIAUgBPAFUATgBEAF8ARgBJAFgAIgAsACIAQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVAAiAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAFkATQBEACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABGAE8AUgBNAEEAVABfAEEAUwBfAEwASQBTAFQAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBvAG4AdgBlAHIAdABzACAAYQAgAGwAaQBzAHQAIABvAGYAIAB2AGEAbAB1AGUAcwAgAGkAbgB0AG8AIABhACAAcwB5AG4AdABhAGMAdABpAGMAYQBsAGwAeQAgAHYAYQBsAGkAZAAgAEUAeABjAGUAbAAgAGEAcgByAGEAeQAgAGMAbwBuAHMAdABhAG4AdAAgAHMAdAByAGkAbgBnACwAXABuACAAIAAgAHUAcwBlAGYAdQBsACAAZgBvAHIAIABlAG0AYgBlAGQAZABpAG4AZwAgAGQAaQByAGUAYwB0AGwAeQAgAGkAbgAgAEwAQQBNAEIARABBACAAZABlAGYAaQBuAGkAdABpAG8AbgBzACAAYQBzACAAewBpAHQAZQBtADEALAAgAGkAdABlAG0AMgAsACAALgAuAC4AfQAgAG8AcgAgAHsAaQB0AGUAbQAxADsAIABpAHQAZQBtADIAOwAgAC4ALgAuAH0ALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIAByAGEAbgBnAGUAIAAgACAAOgAgAFQAaABlACAAbABpAHMAdAAgAG8AcgAgAGEAcgByAGEAeQAgAHQAbwAgAGYAbwByAG0AYQB0AFwAbgAgACAAIAAtACAAWwBmAG8AcgBtAGEAdABdADoAIABPAHAAdABpAG8AbgBhAGwALgAgADAAIAA9ACAAYwBvAG0AbQBhAC0AcwBlAHAAYQByAGEAdABlAGQAIAAoAGgAbwByAGkAegBvAG4AdABhAGwAKQAsACAAMQAgAD0AIABzAGUAbQBpAGMAbwBsAG8AbgAtAHMAZQBwAGEAcgBhAHQAZQBkACAAKAB2AGUAcgB0AGkAYwBhAGwAKQBcAG4AIAAgACAALQAgAFsAcwB0AHkAbABlAF0AIAA6ACAATwBwAHQAaQBvAG4AYQBsAC4AIAAwACAAPQAgAGkAbgBjAGwAdQBkAGUAIABjAHUAcgBsAHkAIABiAHIAYQBjAGUAcwAgACgAZABlAGYAYQB1AGwAdAApACwAIAAxACAAPQAgAG8AbQBpAHQAIABiAHIAYQBjAGUAcwBcAG4AIAAgACAALQAgAFsAcwBvAHIAdABdACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsAC4AIAAwACAAPQAgAG4AbwAgAHMAbwByAHQAIAAoAGQAZQBmAGEAdQBsAHQAKQAsACAAMQAgAD0AIABhAGwAcABoAGEAYgBlAHQAaQBjAGEAbABsAHkAIABzAG8AcgB0AGUAZABcAG4AIAAgACAALQAgAFsAbQBvAGQAZQBdACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsAC4AIAAwACAAPQAgAGkAbgBjAGwAdQBkAGUAIABhAGwAbAAgAHYAYQBsAHUAZQBzACAAKABkAGUAZgBhAHUAbAB0ACkALAAgADEAIAA9ACAAdQBzAGUAIABvAG4AbAB5ACAAdQBuAGkAcQB1AGUAIAB2AGEAbAB1AGUAcwBcAG4AXABuACAAIAAgAE8AdQB0AHAAdQB0ADoAXABuACAAIAAgAC0AIABBACAAcwB0AHIAaQBuAGcAIABmAG8AcgBtAGEAdAB0AGUAZAAgAGEAcwAgAGEAIAB2AGEAbABpAGQAIABFAHgAYwBlAGwAIABhAHIAcgBhAHkAIABjAG8AbgBzAHQAYQBuAHQAXABuACoALwBcAG4AXABuAEYATwBSAE0AQQBUAF8AQQBTAF8ATABJAFMAVAAgAD0AIABMAEEATQBCAEQAQQAoAHIAYQBuAGcAZQAsACAAWwBmAG8AcgBtAGEAdABdACwAIABbAHMAdAB5AGwAZQBdACwAIABbAHMAbwByAHQAXQAsACAAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAATgBvAHIAbQBhAGwAaQB6AGUAIABpAG4AcAB1AHQAIABmAGwAYQBnAHMAIAB3AGkAdABoACAAZABlAGYAYQB1AGwAdAAgAGYAYQBsAGwAYgBhAGMAawBzAFwAbgAgACAAIAAgACAAIAAgACAAcwB0AHkAbABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAHMAdAB5AGwAZQApACwAIABzAHQAeQBsAGUAIAA+ACAAMQApACwAIAAwACwAIABzAHQAeQBsAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZgBvAHIAbQBhAHQALAAgAEkARgAoAE8AUgAoAEkAUwBPAE0ASQBUAFQARQBEACgAZgBvAHIAbQBhAHQAKQAsACAAZgBvAHIAbQBhAHQAIAA+ACAAMQApACwAIAAwACwAIABmAG8AcgBtAGEAdAApACwAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcwBvAHIAdAAsACAASQBGACgATwBSACgASQBTAE8ATQBJAFQAVABFAEQAKABzAG8AcgB0ACkALAAgAHMAbwByAHQAIAA+ACAAMQApACwAIAAwACwAIABzAG8AcgB0ACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAGgAbwBvAHMAZQAgAGEAcgByAGEAeQAgAHMAZQBwAGEAcgBhAHQAbwByACAAYgBhAHMAZQBkACAAbwBuACAAZgBvAHIAbQBhAHQAXABuACAAIAAgACAAIAAgACAAIABzAGUAcABhAHIAYQB0AG8AcgAsACAASQBGACgAZgBvAHIAbQBhAHQAIAA9ACAAMAAsACAAXAAiACwAIABcACIALAAgAFwAIgA7ACAAXAAiACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbgB2AGUAcgB0ACAAdABvACAAMQBEACAAYQByAHIAYQB5ACAAYQBuAGQAIABhAHAAcABsAHkAIAB1AG4AaQBxAHUAZQBuAGUAcwBzACAAbQBvAGQAZQBcAG4AIAAgACAAIAAgACAAIAAgAGwAaQBzAHQALAAgAFMAVwBJAFQAQwBIACgAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAwACwAIABUAE8AQwBPAEwAKAByAGEAbgBnAGUALAAgADMAKQAsACAAIAAgACAAIAAvAC8AIABhAGwAbAAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAxACwAIABVAE4ASQBRAFUARQAoAFQATwBDAE8ATAAoAHIAYQBuAGcAZQAsACAAMwApACkAIAAvAC8AIAB1AG4AaQBxAHUAZQAgAHYAYQBsAHUAZQBzACAAbwBuAGwAeQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAbAB5ACAAcwBvAHIAdAAgAHQAaABlACAAbABpAHMAdABcAG4AIAAgACAAIAAgACAAIAAgAHMAbwByAHQAZQBkACwAIABTAFcASQBUAEMASAAoAHMAbwByAHQALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMAAsACAAbABpAHMAdAAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAbgBvACAAcwBvAHIAdABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAUwBPAFIAVAAoAGwAaQBzAHQAKQAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAYQBsAHAAaABhAGIAZQB0AGkAYwBhAGwAIABzAG8AcgB0AFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEYAaQBuAGEAbAAgAGEAcwBzAGUAbQBiAGwAeQA6ACAAdwByAGEAcAAgAHcAaQB0AGgAIABiAHIAYQBjAGUAcwAgAGkAZgAgAHMAdAB5AGwAZQAgAD0AIAAwAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAFMAVwBJAFQAQwBIACgAcwB0AHkAbABlACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgADAALAAgAFwAIgB7AFwAIgAgACYAIABUAEUAWABUAEoATwBJAE4AKABzAGUAcABhAHIAYQB0AG8AcgAsACAALAAgAHMAbwByAHQAZQBkACkAIAAmACAAXAAiAH0AXAAiACwAIAAgAC8ALwAgAGkAbgBjAGwAdQBkAGUAIABiAHIAYQBjAGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAMQAsACAAVABFAFgAVABKAE8ASQBOACgAcwBlAHAAYQByAGEAdABvAHIALAAgACwAIABzAG8AcgB0AGUAZAApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAG8AbQBpAHQAIABiAHIAYQBjAGUAcwBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUgBFAEMASQBQADoAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAcgBlAGMAaQBwAHIAbwBjAGEAbAAgACgAbQB1AGwAdABpAHAAbABpAGMAYQB0AGkAdgBlACAAaQBuAHYAZQByAHMAZQApACAAbwBmACAAYQAgAG4AdQBtAGIAZQByAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAEEAIABzAGkAbgBnAGwAZQAgAGQAZQBjAGkAbQBhAGwAIAB2AGEAbAB1AGUAIABlAHEAdQBhAGwAIAB0AG8AIAAxACAAZABpAHYAaQBkAGUAZAAgAGIAeQAgAHQAaABlACAAaQBuAHAAdQB0AC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABpAG4AcAB1AHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBAG4AeQAgAG4AbwBuAHoAZQByAG8AIABuAHUAbQBlAHIAaQBjACAAdgBhAGwAdQBlAC4AXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFIAZQB0AHUAcgBuAHMAIABgACMARABJAFYALwAwACEAYAAgAGkAZgAgAGkAbgBwAHUAdAAgAGkAcwAgAHoAZQByAG8ALgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABmAGwAaQBwAHAAaQBuAGcAIABmAHIAYQBjAHQAaQBvAG4AcwAsACAAYwBvAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGUAcwAgACgAZQAuAGcALgAsACAASAB6ACAAlCEgAHMAZQBjAG8AbgBkAHMAKQAsACAAbwByACAAaQBuAHYAZQByAHQAaQBuAGcAIAByAGEAdABpAG8AcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIAAgACAAUgBFAEMASQBQACgANAApACAAkiEgADAALgAyADUAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAAwAC4AMgApACAAkiEgADUAXABuACoALwBcAG4AUgBFAEMASQBQACAAPQAgAEwAQQBNAEIARABBACgAaQBuAHAAdQB0ACwAIAAxACAALwAgAGkAbgBwAHUAdAApADsAXABuAFwAbgAvACoAIABGAFIAQQBDADoAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgACgAbgBvAG4ALQBpAG4AdABlAGcAZQByACkAIABwAGEAcgB0ACAAbwBmACAAYQAgAG4AdQBtAGIAZQByAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAEEAIABzAGMAYQBsAGEAcgAgAGQAZQBjAGkAbQBhAGwAIABiAGUAdAB3AGUAZQBuACAAMAAgAGEAbgBkACAAMQAgACgAbwByACAALQAxACAAYQBuAGQAIAAwACAAaQBmACAAcwBpAGcAbgAgAGkAcwAgAHAAcgBlAHMAZQByAHYAZQBkACkALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAbgB1AG0AYgBlAHIAIAB0AG8AIABlAHgAdAByAGEAYwB0ACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGYAcgBvAG0ALgBcAG4AIAAgACAALQAgAG0AbwBkAGUAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABPAHUAdABwAHUAdAAgAG0AbwBkAGUAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMAApAFwAbgAgACAAIAAgACAAIAAgAC0AIAAwADoAIABBAGwAdwBhAHkAcwAgAHIAZQB0AHUAcgBuACAAcABvAHMAaQB0AGkAdgBlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAXABuACAAIAAgACAAIAAgACAALQAgADEAOgAgAFAAcgBlAHMAZQByAHYAZQAgAHMAaQBnAG4AIABvAGYAIABpAG4AcAB1AHQAIAAoAGUALgBnAC4ALAAgAC0AMwAuADIANQAgAJIhIAAtADAALgAyADUAKQBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAQwBvAG0AcABsAGUAbQBlAG4AdABzACAARQB4AGMAZQBsABkgcwAgAFQAUgBVAE4AQwAgAGEAbgBkACAAUQBVAE8AVABJAEUATgBUACAAZgB1AG4AYwB0AGkAbwBuAHMALgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABkAGUAdABlAGMAdABpAG4AZwAgAGQAZQBjAGkAbQBhAGwAIAByAGUAbQBhAGkAbgBkAGUAcgBzACAAYQBuAGQAIABhAG4AYQBsAHkAegBpAG4AZwAgAG8AZgBmAHMAZQB0AHMAIABmAHIAbwBtACAAdwBoAG8AbABlACAAdgBhAGwAdQBlAHMALgBcAG4AIAAgACAALQAgAFMAaQBnAG4ALQBwAHIAZQBzAGUAcgB2AGkAbgBnACAAbQBvAGQAZQAgAGMAYQBuACAAaQBuAGQAaQBjAGEAdABlACAAdwBoAGUAdABoAGUAcgAgAGEAIAB2AGEAbAB1AGUAIABpAHMAIABqAHUAcwB0ACAAYQBiAG8AdgBlACAAbwByACAAagB1AHMAdAAgAGIAZQBsAG8AdwAgAGEAbgAgAGkAbgB0AGUAZwBlAHIALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIABGAFIAQQBDACgALQAzAC4AMgA1ACkAIAAgACAAIAAgACAAIACSISAAMAAuADIANQAgACAAXABuACAAIAAgAEYAUgBBAEMAKAAtADMALgAyADUALAAgADEAKQAgACAAIAAgAJIhIAAtADAALgAyADUAXABuACoALwBcAG4ARgBSAEEAQwAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARABlAGYAYQB1AGwAdAAgAG0AbwBkAGUAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAGkAbgB2AGEAbABpAGQAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABiAHkAIABzAHUAYgB0AHIAYQBjAHQAaQBuAGcAIABpAG4AdABlAGcAZQByACAAcABvAHIAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAcgBhAGMAXwBwAGEAcgB0ACwAIABpAG4AcAB1AHQAIAAtACAAVABSAFUATgBDACgAaQBuAHAAdQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAUgBlAHQAdQByAG4AIABzAGkAZwBuAGUAZAAgAG8AcgAgAGEAYgBzAG8AbAB1AHQAZQAgAHYAYQBsAHUAZQAgAGQAZQBwAGUAbgBkAGkAbgBnACAAbwBuACAAbQBvAGQAZQBcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAMQAsACAAZgByAGEAYwBfAHAAYQByAHQALAAgAEEAQgBTACgAZgByAGEAYwBfAHAAYQByAHQAKQApAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAFIATwBPAFQAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIAB4AC0AdABoACAAcgBvAG8AdAAgAG8AZgAgAGEAIABuAHUAbQBiAGUAcgAgACgAbwByACAAcwBxAHUAYQByAGUAIAByAG8AbwB0ACAAaQBmACAAbgBvACAAZABlAGcAcgBlAGUAIABpAHMAIABzAHAAZQBjAGkAZgBpAGUAZAApAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAEEAIAByAGUAYQBsACAAZABlAGMAaQBtAGEAbAAgAG4AdQBtAGIAZQByACAAcgBlAHAAcgBlAHMAZQBuAHQAaQBuAGcAIAB0AGgAZQAgAHIAbwBvAHQAIABvAGYAIABgAG4AYAAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbgAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAbgB1AG0AYgBlAHIAIAB0AG8AIAB0AGEAawBlACAAdABoAGUAIAByAG8AbwB0ACAAbwBmAC4AXABuACAAIAAgAC0AIAB4ACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAAVABoAGUAIAByAG8AbwB0ACAAZABlAGcAcgBlAGUALgAgAEQAZQBmAGEAdQBsAHQAcwAgAHQAbwAgADIAIAAoAHMAcQB1AGEAcgBlACAAcgBvAG8AdAApAC4AXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFIAZQBqAGUAYwB0AHMAIABhAGwAbAAgAG4AZQBnAGEAdABpAHYAZQAgAGkAbgBwAHUAdAAgAHYAYQBsAHUAZQBzACAAZgBvAHIAIABgAG4AYAAsACAAcgBlAGcAYQByAGQAbABlAHMAcwAgAG8AZgAgAHIAbwBvAHQALgBcAG4AIAAgACAALQAgAE0AaQBtAGkAYwBzACAARQB4AGMAZQBsACcAcwAgAGIAZQBoAGEAdgBpAG8AcgAgACgAcgBlAHQAdQByAG4AcwAgACMATgBVAE0AIQAgAGkAZgAgAHIAbwBvAHQAIAB3AG8AdQBsAGQAIABiAGUAIABjAG8AbQBwAGwAZQB4ACkALgBcAG4AIAAgACAALQAgAFUAcwBlACAARQB4AGMAZQBsABkgcwAgAGAASQBNAFAATwBXAEUAUgBgACAAbwByACAAYABJAE0AUwBRAFIAVABgACAAZgBvAHIAIABjAG8AbQBwAGwAZQB4ACAAbgB1AG0AYgBlAHIAIABzAHUAcABwAG8AcgB0AC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlAHMAOgBcAG4AIAAgACAAUgBPAE8AVAAoADEANgApACAAIAAgACAAIAAgACAAkiEgADQAXABuACAAIAAgAFIATwBPAFQAKAAyADcALAAgADMAKQAgACAAIAAgAJIhIAAzAFwAbgAgACAAIABSAE8ATwBUACgAOQAsACAAMAAuADUAKQAgACAAIACSISAAOAAxAFwAbgAgACAAIABSAE8ATwBUACgALQA1ACwAIAAzACkAIAAgACAAIACSISAAIwBOAFUATQAhAFwAbgAqAC8AXABuAFIATwBPAFQAIAA9ACAATABBAE0AQgBEAEEAKABuACwAIABbAHgAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAByAG8AbwB0AF8AZABlAGcAcgBlAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAeAApACwAIAAyACwAIAB4ACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABuACAAPAAgADAALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAUwBRAFIAVAAoAC0AMQApACwAIAAvAC8AIABUAHIAaQBnAGcAZQByAHMAIAAjAE4AVQBNACEAIABlAHIAcgBvAHIAIABmAG8AcgAgAG4AZQBnAGEAdABpAHYAZQAgAGIAYQBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AIABeACAAKAAxACAALwAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVABcAG4AIAAgACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAYQAgAG8AbgBlAC0AbABpAG4AZQAsACAAbABhAGIAZQBsAGUAZAAgAHYAZQByAHMAaQBvAG4AIABvAGYAIAB0AGgAZQAgAGYAbwByAG0AdQBsAGEAIABpAG4AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAGMAZQBsAGwALABcAG4AIAAgACAAbwBtAGkAdAB0AGkAbgBnACAAdABoAGUAIABsAGUAYQBkAGkAbgBnACAAZQBxAHUAYQBsACAAcwBpAGcAbgAgAGEAbgBkACAAcAByAGUAcABlAG4AZABpAG4AZwAgAHQAaABlACAAYwBlAGwAbAAgAHIAZQBmAGUAcgBlAG4AYwBlAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABjAGUAbABsACkAXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgACAAIABjAGUAbABsACAAOgAgAEEAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAbwAgAGEAIABjAGUAbABsACAAYwBvAG4AdABhAGkAbgBpAG4AZwAgAGEAIABmAG8AcgBtAHUAbABhAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgACAAIABBACAAcwBpAG4AZwBsAGUALQBsAGkAbgBlACAAcwB0AHIAaQBuAGcAIABpAG4AIAB0AGgAZQAgAGYAbwByAG0AYQB0ACAAXAAiAEEAMQA6AD0AIABGAE8AUgBNAFUATABBACgALgAuAC4AKQBcACIAXABuACAAIAAgACAAIABVAHMAZQBmAHUAbAAgAGYAbwByACAAYQB1AGQAaQB0AGkAbgBnACwAIABkAG8AYwB1AG0AZQBuAHQAYQB0AGkAbwBuACwAIABkAGEAcwBoAGIAbwBhAHIAZABzACwAIABvAHIAIAB0AGUAYQBjAGgAaQBuAGcAIAB0AG8AbwBsAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABCADMAKQAgACAAkiEgAFwAIgBCADMAOgA9ACAAUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAEMANQApACAAIACSISAAXAAiAEMANQA6AD0AIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAzACkAXAAiAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAAVABoAGUAIAByAGUAcwB1AGwAdAAgAGkAcwAgAGUAcQB1AGkAdgBhAGwAZQBuAHQAIAB0AG8AOgAgAEMARQBMAEwAKABcACIAYQBkAGQAcgBlAHMAcwBcACIALAAgAGMAZQBsAGwAKQAgACYAIABcACIAOgA9ACAAXAAiACAAJgAgAFQARQBYAFQAQQBGAFQARQBSACgARgBPAFIATQBVAEwAQQBUAEUAWABUACgAYwBlAGwAbAApACwAIABcACIAPQBcACIAKQBcAG4AIAAgACAAIAAgAC0AIABJAGYAIAB0AGgAZQAgAHIAZQBmAGUAcgBlAG4AYwBlAGQAIABjAGUAbABsACAAZABvAGUAcwAgAG4AbwB0ACAAYwBvAG4AdABhAGkAbgAgAGEAIABmAG8AcgBtAHUAbABhACwAIABhAG4AIABlAHIAcgBvAHIAIAB3AGkAbABsACAAbwBjAGMAdQByAC4AXABuACAAIAAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAGQAbwBlAHMAIABuAG8AdAAgAGUAdgBhAGwAdQBhAHQAZQAgAG8AcgAgAGEAbAB0AGUAcgAgAHQAaABlACAAZgBvAHIAbQB1AGwAYQAUIG8AbgBsAHkAIABmAG8AcgBtAGEAdABzACAAaQB0ACAAZgBvAHIAIABkAGkAcwBwAGwAYQB5AC4AXABuACoALwBcAG4ARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAIAA9ACAATABBAE0AQgBEAEEAKABmAG8AcgBtAHUAbABhAF8AYwBlAGwAbAAsACAALwAvACAAQQAgAHIAZQBmAGUAcgBlAG4AYwBlACAAdABvACAAYQAgAGMAZQBsAGwAIABjAG8AbgB0AGEAaQBuAGkAbgBnACAAYQAgAGYAbwByAG0AdQBsAGEAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHIAYQB3ACwAIABGAE8AUgBNAFUATABBAFQARQBYAFQAKABmAG8AcgBtAHUAbABhAF8AYwBlAGwAbAApACwAIAAvAC8AIABcACIAPQBSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgAGMAbABlAGEAbgAsACAAVABFAFgAVABBAEYAVABFAFIAKAByAGEAdwAsACAAXAAiAD0AXAAiACkALAAgAC8ALwAgAFwAIgBSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAEMARQBMAEwAKABcACIAYQBkAGQAcgBlAHMAcwBcACIALAAgAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgAFwAIgAkAFwAIgAsACAAXAAiAFwAIgApACAAJgAgAFwAIgA6AD0AIABcACIALABcAG4AIAAgACAAIAAgACAAIAAgAGwAYQBiAGUAbAAgACYAIABjAGwAZQBhAG4AXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUgBPAFUATgBEAF8ARgBJAFgAXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAgACAAUgBvAHUAbgBkAHMAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAcwAgAGEAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGEAIABzAHAAZQBjAGkAZgBpAGUAZAAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AXABuACAAIAAgAE8AcAB0AGkAbwBuAGEAbABsAHkAIAByAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAcwB1AGwAdAAgAGEAcwAgAGEAIABmAGkAeABlAGQALQB3AGkAZAB0AGgAIAB0AGUAeAB0ACAAcwB0AHIAaQBuAGcALAAgAHAAcgBlAHMAZQByAHYAaQBuAGcAIAB0AHIAYQBpAGwAaQBuAGcAIAB6AGUAcgBvAHMALgBcAG4AXABuACAAIAAgAFMAeQBuAHQAYQB4ADoAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAG4AdQBtAGIAZQByACwAIABwAGwAYQBjAGUAcwAsACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAbgB1AG0AYgBlAHIAIAAgACAAIAAgACAAOgAgAFQAaABlACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQAgAHQAbwAgAHAAcgBvAGMAZQBzAHMALgBcAG4AIAAgACAAIAAgAHAAbABhAGMAZQBzACAAIAAgACAAIAAgADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAZQB0AGEAaQBuAC4AXABuACAAIAAgACAAIABhAHMAXwB0AGUAeAB0ACAAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgBzACAAbwB1AHQAcAB1AHQAIABhAHMAIAB0AGUAeAB0ACAAKABlAC4AZwAuACwAIABcACIAMwAuADEANAAwAFwAIgApAC4AXABuACAAIAAgACAAIAB1AHMAZQBfAHIAbwB1AG4AZAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIABhAHAAcABsAGkAZQBzACAAcgBvAHUAbgBkAGkAbgBnAC4AIABPAHQAaABlAHIAdwBpAHMAZQAsACAAdAByAHUAbgBjAGEAdABlAHMALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIABuAHUAbQBiAGUAcgAgAG8AcgAgAHQAZQB4AHQAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIAByAG8AdQBuAGQAZQBkACAAbwByACAAdAByAHUAbgBjAGEAdABlAGQAIAB2AGEAbAB1AGUAIAB0AG8AIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAyACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgADMALgAxADQAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADMALAAgAFQAUgBVAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQBcACIAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADQALAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQApACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQA1AFwAIgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABGAEEATABTAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIAAzAC4AMQA0ADEANQA5ADIANgA1ADQAIAAgACAAKABjAGEAcABwAGUAZAAgAHQAbwAgADkAIABkAGUAYwBpAG0AYQBsAHMAKQBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABUAFIAVQBFACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxADUAOQAyADYANQAzADUAOQAwAFwAIgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAgACAALQAgAEUAeABjAGUAbAAgAGwAaQBtAGkAdABzACAAbgB1AG0AZQByAGkAYwAgAGQAaQBzAHAAbABhAHkAIABwAHIAZQBjAGkAcwBpAG8AbgAgAHQAbwAgAH4AOQAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuACAAVwBoAGUAbgAgAGEAcwBfAHQAZQB4AHQAIAA9ACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAIABpAHMAIABjAGEAcABwAGUAZAAgAGEAdAAgADkAIABkAGkAZwBpAHQAcwAgAGYAbwByACAAYwBvAG4AcwBpAHMAdABlAG4AYwB5AC4AXABuACAAIAAgACAAIAAtACAAVABvACAAZABpAHMAcABsAGEAeQAgAGYAdQBsAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgAG8AcgAgAHAAcgBlAHMAZQByAHYAZQAgAHQAcgBhAGkAbABpAG4AZwAgAHoAZQByAG8AcwAsACAAcwBlAHQAIABhAHMAXwB0AGUAeAB0ACAAPQAgAFQAUgBVAEUALgBcAG4AIAAgACAAIAAgAC0AIABTAHUAcABwAG8AcgB0AHMAIABiAG8AdABoACAAcgBvAHUAbgBkAGkAbgBnACAAYQBuAGQAIAB0AHIAdQBuAGMAYQB0AGkAbwBuACAAbQBvAGQAZQBzAC4AXABuACAAIAAgACAAIAAtACAASQBkAGUAYQBsACAAZgBvAHIAIABmAG8AcgBtAGEAdAB0AGkAbgBnACAAYwBvAG4AcwB0AGEAbgB0AHMALAAgAHYAaQBzAHUAYQBsACAAZABpAHMAcABsAGEAeQAgAGMAbwBuAHQAcgBvAGwALAAgAG8AcgAgAGUAbgBzAHUAcgBpAG4AZwAgAGMAbABlAGEAbgAgAG8AdQB0AHAAdQB0AHMAIABpAG4AIAByAGUAcABvAHIAdABzAC4AXABuACoALwBcAG4AUgBPAFUATgBEAF8ARgBJAFgAIAA9ACAATABBAE0AQgBEAEEAKABcAG4AIAAgACAAIABuAHUAbQBiAGUAcgAsACAALwAvACAAUgBlAHEAdQBpAHIAZQBkADoAIAB0AGgAZQAgAG4AdQBtAGIAZQByACAAdABvACAAcgBvAHUAbgBkACAAbwByACAAdAByAHUAbgBjAGEAdABlAFwAbgAgACAAIAAgAHAAbABhAGMAZQBzACwAIAAvAC8AIABSAGUAcQB1AGkAcgBlAGQAOgAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAdABvACAAcgBlAHQAYQBpAG4AXABuACAAIAAgACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgAC8ALwAgAE8AcAB0AGkAbwBuAGEAbAA6ACAAaQBmACAAVABSAFUARQAsACAAcgBlAHQAdQByAG4AIAByAGUAcwB1AGwAdAAgAGEAcwAgAHQAZQB4AHQAIAB3AGkAdABoACAAZgBpAHgAZQBkACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAFwAbgAgACAAIAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQAsACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAG8AdQBuAGQAOwAgAGkAZgAgAEYAQQBMAFMARQAgAG8AcgAgAG8AbQBpAHQAdABlAGQALAAgAHQAcgB1AG4AYwBhAHQAZQBcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAbgAsACAATgAoAG4AdQBtAGIAZQByACkALAAgAC8ALwAgAEUAbgBzAHUAcgBlACAAbgB1AG0AZQByAGkAYwAgAGkAbgBwAHUAdABcAG4AIAAgACAAIAAgACAAIAAgAHIAYQB3AF8AcAAsACAATgAoAHAAbABhAGMAZQBzACkALAAgAC8ALwAgAFIAYQB3ACAAaQBuAHAAdQB0ACAAZgBvAHIAIABwAGwAYQBjAGUAcwBcAG4AIAAgACAAIAAgACAAIAAgAHIAbwB1AG4AZABfAGYAbABhAGcALAAgAEkARgAoAEkAUwBCAEwAQQBOAEsAKAB1AHMAZQBfAHIAbwB1AG4AZAApACwAIABGAEEATABTAEUALAAgAHUAcwBlAF8AcgBvAHUAbgBkACkALABcAG4AIAAgACAAIAAgACAAIAAgAHIAZQB0AHUAcgBuAF8AdABlAHgAdAAsACAASQBGACgASQBTAEIATABBAE4ASwAoAGEAcwBfAHQAZQB4AHQAKQAsACAARgBBAEwAUwBFACwAIABhAHMAXwB0AGUAeAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARQB4AGMAZQBsACAAbwBuAGwAeQAgAHIAZQBsAGkAYQBiAGwAeQAgAGQAaQBzAHAAbABhAHkAcwAgAHUAcAAgAHQAbwAgADkAIABkAGUAYwBpAG0AYQBsAHMAIABhAHMAIABuAHUAbQBlAHIAaQBjAFwAbgAgACAAIAAgACAAIAAgACAAbQBhAHgAXwBwAGwAYQBjAGUAcwAsACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIAByAGEAdwBfAHAALAAgAE0ASQBOACgAcgBhAHcAXwBwACwAIAA5ACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcAB3AHIAXwAxADAALAAgADEAMAAgAF4AIABtAGEAeABfAHAAbABhAGMAZQBzACwAIAAvAC8AIABQAG8AdwBlAHIAIABvAGYAIAAxADAAIABmAG8AcgAgAHIAbwB1AG4AZABpAG4AZwAvAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuACAAIAAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFAAZQByAGYAbwByAG0AIAByAG8AdQBuAGQAaQBuAGcAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAEkARgAoAHIAbwB1AG4AZABfAGYAbABhAGcALAAgAFIATwBVAE4ARAAoAG4ALAAgAG0AYQB4AF8AcABsAGEAYwBlAHMAKQAsACAAVABSAFUATgBDACgAbgAgACoAIABwAHcAcgBfADEAMAApACAALwAgAHAAdwByAF8AMQAwACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAGYAbwByAG0AYQB0ACAAYQBzACAAZgBpAHgAZQBkAC0AbABlAG4AZwB0AGgAIABzAHQAcgBpAG4AZwBcAG4AIAAgACAAIAAgACAAIAAgAGYAaQBuAGEAbAAsACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIABUAEUAWABUACgAcgBlAHMAdQBsAHQALAAgAFwAIgAwAC4AXAAiACAAJgAgAFIARQBQAFQAKABcACIAMABcACIALAAgAG0AYQB4AF8AcABsAGEAYwBlAHMAKQApACwAIAByAGUAcwB1AGwAdAApACwAXABuACAAIAAgACAAIAAgACAAIABmAGkAbgBhAGwAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQwBPAFUATgBUAEEAXwBTAFQAUgBJAEMAVABcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAYQAgAGMAbwB1AG4AdAAgAG8AZgAgAG4AbwBuAC0AYgBsAGEAbgBrACwAIABuAG8AbgAtAGUAbQBwAHQAeQAsACAAYQBuAGQAIABuAG8AbgAtAHcAaABpAHQAZQBzAHAAYQBjAGUALQBvAG4AbAB5ACAAdgBhAGwAdQBlAHMAIABmAHIAbwBtACAAYQAgAHIAYQBuAGcAZQAuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAMAAgAGkAZgAgAG4AbwAgAG0AZQBhAG4AaQBuAGcAZgB1AGwAIABjAG8AbgB0AGUAbgB0ACAAZQB4AGkAcwB0AHMALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIABpAG4AcAB1AHQAIAA6ACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAHIAIABhAG4AeQAgAHMAaQBuAGcAbABlAC0AYwBvAGwAdQBtAG4AIAByAGEAbgBnAGUAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABJAG4AdABlAGcAZQByADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGMAZQBsAGwAcwAgAHQAaABhAHQAIABjAG8AbgB0AGEAaQBuACAAbQBlAGEAbgBpAG4AZwBmAHUAbAAgAGMAbwBuAHQAZQBuAHQAIAAoAGkAZwBuAG8AcgBlAHMAIABcACIAXAAiACwAIABcACIAIABcACIAKQBcAG4AXABuACAAIAAgAEIAZQBoAGEAdgBpAG8AcgA6AFwAbgAgACAAIAAtACAASQBmACAAdABoAGUAIAByAGEAbgBnAGUAIABjAG8AbgB0AGEAaQBuAHMAIABvAG4AbAB5ACAAYgBsAGEAbgBrAHMAIABvAHIAIAB3AGgAaQB0AGUAcwBwAGEAYwBlAC0AbwBuAGwAeQAgAGMAZQBsAGwAcwAgAJIhIAByAGUAdAB1AHIAbgBzACAAMABcAG4AIAAgACAALQAgAE8AdABoAGUAcgB3AGkAcwBlACAAcgBlAHQAdQByAG4AcwAgAEMATwBVAE4AVABBACgAaQBuAHAAdQB0ACkAXABuACAAIAAgAC0AIABBAHMAcwB1AG0AZQBzACAAaQBuAHAAdQB0ACAAaQBzACAAYQAgAHMAdABhAHQAaQBjACAAbwByACAAcwB0AHIAdQBjAHQAdQByAGUAZAAgAHIAYQBuAGcAZQAgACgAbgBvAHQAIABkAHkAbgBhAG0AaQBjACAAcwBwAGkAbABsACkAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEMATwBVAE4AVABBAF8AUwBUAFIASQBDAFQAKAB7AFwAIgBhAHAAcABsAGUAXAAiACwAIABcACIAXAAiACwAIABcACIAIABcACIALAAgAFwAIgBnAHIAYQBwAGUAXAAiAH0AKQAgAJIhIAAyAFwAbgAqAC8AXABuAEMATwBVAE4AVABBAF8AUwBUAFIASQBDAFQAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgAEkARgAoAEMATwBVAE4AVABJAEYAKABpAG4AcAB1AHQALAAgAFwAIgAqAD8AXAAiACkAIAA9ACAAMAAsACAAMAAsACAAQwBPAFUATgBUAEEAKABpAG4AcAB1AHQAKQApACkAOwAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBGAE8AUgBNAEEAVABfAEEAUwBfAEwASQBTAFQAIgAsACIAUgBFAEMASQBQACIALAAiAEYAUgBBAEMAIgAsACIAUgBPAE8AVAAiACwAIgBGAE8AUgBNAFUATABBAF8AVABFAFgAVAAiACwAIgBSAE8AVQBOAEQAXwBGAEkAWAAiACwAIgBDAE8AVQBOAFQAQQBfAFMAVABSAEkAQwBUACIAXQAsACIAbABvAGMAYQBsAGUAIgA6AHsAIgBsAGkAcwB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAcgBvAHcAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBjAG8AbAB1AG0AbgBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUABvAHMAaQB0AGkAbwBuAHMAIgA6AFsAMwBdACwAIgBkAGUAYwBpAG0AYQBsAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiAC4AIgAsACIAZABhAHQAZQBPAHIAZABlAHIAIgA6ACIAWQBNAEQAIgAsACIAYwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsACIAOgAiACQAIgAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbABMAGUAYQBkACIAOgB0AHIAdQBlACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAZQBwAEIAeQBTAHAAYQBjAGUAIgA6AGYAYQBsAHMAZQAsACIAcgBvAHcATABlAHQAdABlAHIAIgA6ACIAUgAiACwAIgBjAG8AbAB1AG0AbgBMAGUAdAB0AGUAcgAiADoAIgBDACIALAAiAHIAYwBMAGUAZgB0AEIAcgBhAGMAawBlAHQAIgA6ACIAWwAiACwAIgByAGMAUgBpAGcAaAB0AEIAcgBhAGMAawBlAHQAIgA6ACIAXQAiACwAIgBzAHQAYQB0AGUAbQBlAG4AdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGwAbwBjAGEAbABlAE4AYQBtAGUAIgA6ACIAZQBuAC0AdQBzACIAfQB9AA==</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>